<commit_message>
add ANC HIV prevalence
</commit_message>
<xml_diff>
--- a/Config/Calibration_targets_Kenya.xlsx
+++ b/Config/Calibration_targets_Kenya.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11700"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17865" windowHeight="8250"/>
   </bookViews>
   <sheets>
     <sheet name="Calibration" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="47">
   <si>
     <t>N</t>
   </si>
@@ -153,6 +153,18 @@
   </si>
   <si>
     <t>DeVuyst 2012; BJC</t>
+  </si>
+  <si>
+    <t>HIV prevalence in women - ANC</t>
+  </si>
+  <si>
+    <t>ANC Surveillance Report 2011</t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prevalence estimates were reported in ANC surveillance report 2011. The number of HIV positive women and the number of women attending ANC each year were not available, except for 2011. The number positive each year from 1990-2003 were calculated using the number of women attending ANC in 2011.  </t>
   </si>
 </sst>
 </file>
@@ -521,8 +533,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1785,163 +1797,418 @@
       <c r="J43" t="s">
         <v>30</v>
       </c>
+      <c r="K43" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A44" s="1"/>
-      <c r="B44" s="1"/>
-      <c r="C44" s="1"/>
-      <c r="D44" s="1"/>
-      <c r="E44" s="1"/>
-      <c r="F44" s="1"/>
-      <c r="G44" s="6"/>
+      <c r="A44" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D44" s="1">
+        <v>1990</v>
+      </c>
+      <c r="E44" s="1">
+        <f>Table1[[#This Row],[Mean]]*Table1[[#This Row],[N]]</f>
+        <v>73.8</v>
+      </c>
+      <c r="F44" s="1">
+        <v>410</v>
+      </c>
+      <c r="G44" s="6">
+        <v>0.18</v>
+      </c>
       <c r="H44" s="7"/>
       <c r="I44" s="7"/>
+      <c r="J44" t="s">
+        <v>30</v>
+      </c>
       <c r="K44" s="8"/>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A45" s="1"/>
-      <c r="B45" s="1"/>
-      <c r="C45" s="1"/>
-      <c r="D45" s="1"/>
-      <c r="E45" s="1"/>
-      <c r="F45" s="1"/>
-      <c r="G45" s="6"/>
+      <c r="A45" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D45" s="1">
+        <v>1991</v>
+      </c>
+      <c r="E45" s="1">
+        <f>Table1[[#This Row],[Mean]]*Table1[[#This Row],[N]]</f>
+        <v>73.8</v>
+      </c>
+      <c r="F45" s="1">
+        <v>410</v>
+      </c>
+      <c r="G45" s="6">
+        <v>0.18</v>
+      </c>
       <c r="H45" s="7"/>
       <c r="I45" s="7"/>
+      <c r="J45" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A46" s="1"/>
-      <c r="B46" s="1"/>
-      <c r="C46" s="1"/>
-      <c r="D46" s="1"/>
-      <c r="E46" s="1"/>
-      <c r="F46" s="1"/>
-      <c r="G46" s="6"/>
+      <c r="A46" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D46" s="1">
+        <v>1992</v>
+      </c>
+      <c r="E46" s="1">
+        <f>Table1[[#This Row],[Mean]]*Table1[[#This Row],[N]]</f>
+        <v>77.900000000000006</v>
+      </c>
+      <c r="F46" s="1">
+        <v>410</v>
+      </c>
+      <c r="G46" s="6">
+        <v>0.19</v>
+      </c>
       <c r="H46" s="7"/>
       <c r="I46" s="7"/>
+      <c r="J46" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A47" s="1"/>
-      <c r="B47" s="1"/>
-      <c r="C47" s="1"/>
-      <c r="D47" s="1"/>
-      <c r="E47" s="1"/>
-      <c r="F47" s="1"/>
-      <c r="G47" s="6"/>
+      <c r="A47" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D47" s="1">
+        <v>1993</v>
+      </c>
+      <c r="E47" s="1">
+        <f>Table1[[#This Row],[Mean]]*Table1[[#This Row],[N]]</f>
+        <v>77.900000000000006</v>
+      </c>
+      <c r="F47" s="1">
+        <v>410</v>
+      </c>
+      <c r="G47" s="6">
+        <v>0.19</v>
+      </c>
       <c r="H47" s="7"/>
       <c r="I47" s="7"/>
+      <c r="J47" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A48" s="1"/>
-      <c r="B48" s="1"/>
-      <c r="C48" s="1"/>
-      <c r="D48" s="1"/>
-      <c r="E48" s="1"/>
-      <c r="F48" s="1"/>
-      <c r="G48" s="6"/>
+      <c r="A48" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D48" s="1">
+        <v>1994</v>
+      </c>
+      <c r="E48" s="1">
+        <f>Table1[[#This Row],[Mean]]*Table1[[#This Row],[N]]</f>
+        <v>118.89999999999999</v>
+      </c>
+      <c r="F48" s="1">
+        <v>410</v>
+      </c>
+      <c r="G48" s="6">
+        <v>0.28999999999999998</v>
+      </c>
       <c r="H48" s="7"/>
       <c r="I48" s="7"/>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A49" s="1"/>
-      <c r="B49" s="1"/>
-      <c r="C49" s="1"/>
-      <c r="D49" s="1"/>
-      <c r="E49" s="1"/>
-      <c r="F49" s="1"/>
-      <c r="G49" s="6"/>
+      <c r="J48" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D49" s="1">
+        <v>1995</v>
+      </c>
+      <c r="E49" s="1">
+        <f>Table1[[#This Row],[Mean]]*Table1[[#This Row],[N]]</f>
+        <v>98.399999999999991</v>
+      </c>
+      <c r="F49" s="1">
+        <v>410</v>
+      </c>
+      <c r="G49" s="6">
+        <v>0.24</v>
+      </c>
       <c r="H49" s="7"/>
       <c r="I49" s="7"/>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A50" s="1"/>
-      <c r="B50" s="1"/>
-      <c r="C50" s="1"/>
-      <c r="D50" s="1"/>
-      <c r="E50" s="1"/>
-      <c r="F50" s="1"/>
-      <c r="G50" s="6"/>
+      <c r="J49" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D50" s="1">
+        <v>1996</v>
+      </c>
+      <c r="E50" s="1">
+        <f>Table1[[#This Row],[Mean]]*Table1[[#This Row],[N]]</f>
+        <v>106.60000000000001</v>
+      </c>
+      <c r="F50" s="1">
+        <v>410</v>
+      </c>
+      <c r="G50" s="6">
+        <v>0.26</v>
+      </c>
       <c r="H50" s="7"/>
       <c r="I50" s="7"/>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A51" s="1"/>
-      <c r="B51" s="1"/>
-      <c r="C51" s="1"/>
-      <c r="D51" s="1"/>
-      <c r="E51" s="1"/>
-      <c r="F51" s="1"/>
-      <c r="G51" s="6"/>
+      <c r="J50" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D51" s="1">
+        <v>1997</v>
+      </c>
+      <c r="E51" s="1">
+        <f>Table1[[#This Row],[Mean]]*Table1[[#This Row],[N]]</f>
+        <v>131.19999999999999</v>
+      </c>
+      <c r="F51" s="1">
+        <v>410</v>
+      </c>
+      <c r="G51" s="6">
+        <v>0.32</v>
+      </c>
       <c r="H51" s="7"/>
       <c r="I51" s="7"/>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A52" s="1"/>
-      <c r="B52" s="1"/>
-      <c r="C52" s="1"/>
-      <c r="D52" s="1"/>
-      <c r="E52" s="1"/>
-      <c r="F52" s="1"/>
-      <c r="G52" s="6"/>
+      <c r="J51" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D52" s="1">
+        <v>1998</v>
+      </c>
+      <c r="E52" s="1">
+        <f>Table1[[#This Row],[Mean]]*Table1[[#This Row],[N]]</f>
+        <v>110.7</v>
+      </c>
+      <c r="F52" s="1">
+        <v>410</v>
+      </c>
+      <c r="G52" s="6">
+        <v>0.27</v>
+      </c>
       <c r="H52" s="7"/>
       <c r="I52" s="7"/>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A53" s="1"/>
-      <c r="B53" s="1"/>
-      <c r="C53" s="1"/>
-      <c r="D53" s="1"/>
-      <c r="E53" s="1"/>
-      <c r="F53" s="1"/>
-      <c r="G53" s="6"/>
+      <c r="J52" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D53" s="1">
+        <v>1999</v>
+      </c>
+      <c r="E53" s="1">
+        <f>Table1[[#This Row],[Mean]]*Table1[[#This Row],[N]]</f>
+        <v>102.5</v>
+      </c>
+      <c r="F53" s="1">
+        <v>410</v>
+      </c>
+      <c r="G53" s="6">
+        <v>0.25</v>
+      </c>
       <c r="H53" s="7"/>
       <c r="I53" s="7"/>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A54" s="1"/>
-      <c r="B54" s="1"/>
-      <c r="C54" s="1"/>
-      <c r="D54" s="1"/>
-      <c r="E54" s="1"/>
-      <c r="F54" s="1"/>
-      <c r="G54" s="6"/>
+      <c r="J53" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D54" s="1">
+        <v>2000</v>
+      </c>
+      <c r="E54" s="1">
+        <f>Table1[[#This Row],[Mean]]*Table1[[#This Row],[N]]</f>
+        <v>135.30000000000001</v>
+      </c>
+      <c r="F54" s="1">
+        <v>410</v>
+      </c>
+      <c r="G54" s="6">
+        <v>0.33</v>
+      </c>
       <c r="H54" s="7"/>
       <c r="I54" s="7"/>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A55" s="1"/>
-      <c r="B55" s="1"/>
-      <c r="C55" s="1"/>
-      <c r="D55" s="1"/>
-      <c r="E55" s="1"/>
-      <c r="F55" s="1"/>
-      <c r="G55" s="6"/>
+      <c r="J54" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D55" s="1">
+        <v>2001</v>
+      </c>
+      <c r="E55" s="1">
+        <f>Table1[[#This Row],[Mean]]*Table1[[#This Row],[N]]</f>
+        <v>118.89999999999999</v>
+      </c>
+      <c r="F55" s="1">
+        <v>410</v>
+      </c>
+      <c r="G55" s="6">
+        <v>0.28999999999999998</v>
+      </c>
       <c r="H55" s="7"/>
       <c r="I55" s="7"/>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A56" s="1"/>
-      <c r="B56" s="1"/>
-      <c r="C56" s="1"/>
-      <c r="D56" s="1"/>
-      <c r="E56" s="1"/>
-      <c r="F56" s="1"/>
-      <c r="G56" s="6"/>
+      <c r="J55" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D56" s="1">
+        <v>2002</v>
+      </c>
+      <c r="E56" s="1">
+        <f>Table1[[#This Row],[Mean]]*Table1[[#This Row],[N]]</f>
+        <v>106.60000000000001</v>
+      </c>
+      <c r="F56" s="1">
+        <v>410</v>
+      </c>
+      <c r="G56" s="6">
+        <v>0.26</v>
+      </c>
       <c r="H56" s="7"/>
       <c r="I56" s="7"/>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A57" s="1"/>
-      <c r="B57" s="1"/>
-      <c r="C57" s="1"/>
-      <c r="D57" s="1"/>
-      <c r="E57" s="1"/>
-      <c r="F57" s="1"/>
-      <c r="G57" s="6"/>
+      <c r="J56" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D57" s="1">
+        <v>2003</v>
+      </c>
+      <c r="E57" s="1">
+        <f>Table1[[#This Row],[Mean]]*Table1[[#This Row],[N]]</f>
+        <v>106.60000000000001</v>
+      </c>
+      <c r="F57" s="1">
+        <v>410</v>
+      </c>
+      <c r="G57" s="6">
+        <v>0.26</v>
+      </c>
       <c r="H57" s="7"/>
       <c r="I57" s="7"/>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J57" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" s="1"/>
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
@@ -1952,7 +2219,7 @@
       <c r="H58" s="7"/>
       <c r="I58" s="7"/>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" s="1"/>
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
@@ -1963,7 +2230,7 @@
       <c r="H59" s="7"/>
       <c r="I59" s="7"/>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" s="1"/>
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
@@ -1974,7 +2241,7 @@
       <c r="H60" s="7"/>
       <c r="I60" s="7"/>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" s="1"/>
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
@@ -1985,7 +2252,7 @@
       <c r="H61" s="7"/>
       <c r="I61" s="7"/>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" s="1"/>
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
@@ -1996,7 +2263,7 @@
       <c r="H62" s="7"/>
       <c r="I62" s="7"/>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" s="1"/>
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>

</xml_diff>

<commit_message>
Update Excel file w/ usage status of calibration data
</commit_message>
<xml_diff>
--- a/Config/Calibration_targets_Kenya.xlsx
+++ b/Config/Calibration_targets_Kenya.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20363"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20364"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\udrive.uw.edu\udrive\Kenya_model_HPV-HIVacq\HHCoM\Config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\HHCoM\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77FBC3E7-4A35-4B22-96AC-7AB4A3DFDF46}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89D5381A-B9E7-486E-9B3F-177201184EF2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9525" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Calibration" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="767" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="870" uniqueCount="84">
   <si>
     <t>Criteria</t>
   </si>
@@ -274,9 +274,6 @@
   </si>
   <si>
     <t>% CIN3 attributable to non-9v HPV</t>
-  </si>
-  <si>
-    <t>N</t>
   </si>
   <si>
     <t xml:space="preserve">Total population size </t>
@@ -806,24 +803,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M174"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A96" sqref="A96"/>
+    <sheetView tabSelected="1" topLeftCell="A106" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F97" sqref="F97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="30.28515625" customWidth="1"/>
     <col min="2" max="2" width="23.42578125" customWidth="1"/>
-    <col min="3" max="3" width="11" style="1" customWidth="1"/>
-    <col min="4" max="4" width="12.42578125" customWidth="1"/>
+    <col min="3" max="3" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7.5703125" customWidth="1"/>
     <col min="6" max="6" width="10.28515625" customWidth="1"/>
     <col min="7" max="7" width="10" customWidth="1"/>
-    <col min="8" max="8" width="11.140625" customWidth="1"/>
+    <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13" style="29" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="10.85546875" customWidth="1"/>
-    <col min="12" max="12" width="9.28515625" customWidth="1"/>
+    <col min="12" max="12" width="15.7109375" customWidth="1"/>
     <col min="13" max="13" width="54.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1132,7 +1129,9 @@
       </c>
       <c r="J10" s="25"/>
       <c r="K10" s="25"/>
-      <c r="L10" s="25"/>
+      <c r="L10" s="25" t="s">
+        <v>18</v>
+      </c>
       <c r="M10" s="25">
         <f>Table1[[#This Row],[n]]/Table1[[#This Row],[Total N]]*100000</f>
         <v>0.71663276482550387</v>
@@ -1170,7 +1169,9 @@
       </c>
       <c r="J11" s="25"/>
       <c r="K11" s="25"/>
-      <c r="L11" s="25"/>
+      <c r="L11" s="25" t="s">
+        <v>18</v>
+      </c>
       <c r="M11" s="25">
         <v>0.84806759505553897</v>
       </c>
@@ -1207,7 +1208,9 @@
       </c>
       <c r="J12" s="25"/>
       <c r="K12" s="25"/>
-      <c r="L12" s="25"/>
+      <c r="L12" s="25" t="s">
+        <v>18</v>
+      </c>
       <c r="M12" s="25">
         <v>7.9909247379126498</v>
       </c>
@@ -1244,7 +1247,9 @@
       </c>
       <c r="J13" s="25"/>
       <c r="K13" s="25"/>
-      <c r="L13" s="25"/>
+      <c r="L13" s="25" t="s">
+        <v>18</v>
+      </c>
       <c r="M13" s="25">
         <v>20.976373024565699</v>
       </c>
@@ -1281,7 +1286,9 @@
       </c>
       <c r="J14" s="25"/>
       <c r="K14" s="25"/>
-      <c r="L14" s="25"/>
+      <c r="L14" s="25" t="s">
+        <v>18</v>
+      </c>
       <c r="M14" s="25">
         <v>40.716632764825398</v>
       </c>
@@ -1318,7 +1325,9 @@
       </c>
       <c r="J15" s="25"/>
       <c r="K15" s="25"/>
-      <c r="L15" s="25"/>
+      <c r="L15" s="25" t="s">
+        <v>18</v>
+      </c>
       <c r="M15" s="25">
         <v>62.664684712877403</v>
       </c>
@@ -1355,7 +1364,9 @@
       </c>
       <c r="J16" s="25"/>
       <c r="K16" s="25"/>
-      <c r="L16" s="25"/>
+      <c r="L16" s="25" t="s">
+        <v>18</v>
+      </c>
       <c r="M16" s="25">
         <v>83.052730402127906</v>
       </c>
@@ -1392,7 +1403,9 @@
       </c>
       <c r="J17" s="25"/>
       <c r="K17" s="25"/>
-      <c r="L17" s="25"/>
+      <c r="L17" s="25" t="s">
+        <v>18</v>
+      </c>
       <c r="M17" s="25">
         <v>103.442340791738</v>
       </c>
@@ -1429,7 +1442,9 @@
       </c>
       <c r="J18" s="25"/>
       <c r="K18" s="25"/>
-      <c r="L18" s="25"/>
+      <c r="L18" s="25" t="s">
+        <v>18</v>
+      </c>
       <c r="M18" s="25">
         <v>130.32389297449501</v>
       </c>
@@ -1466,7 +1481,9 @@
       </c>
       <c r="J19" s="25"/>
       <c r="K19" s="25"/>
-      <c r="L19" s="25"/>
+      <c r="L19" s="25" t="s">
+        <v>18</v>
+      </c>
       <c r="M19" s="25">
         <v>150.45376310436501</v>
       </c>
@@ -1503,7 +1520,9 @@
       </c>
       <c r="J20" s="25"/>
       <c r="K20" s="25"/>
-      <c r="L20" s="25"/>
+      <c r="L20" s="25" t="s">
+        <v>18</v>
+      </c>
       <c r="M20" s="25">
         <v>156.29791894852099</v>
       </c>
@@ -1540,7 +1559,9 @@
       </c>
       <c r="J21" s="25"/>
       <c r="K21" s="25"/>
-      <c r="L21" s="25"/>
+      <c r="L21" s="25" t="s">
+        <v>18</v>
+      </c>
       <c r="M21" s="25">
         <v>150.71350336410501</v>
       </c>
@@ -1577,7 +1598,9 @@
       </c>
       <c r="J22" s="25"/>
       <c r="K22" s="25"/>
-      <c r="L22" s="25"/>
+      <c r="L22" s="25" t="s">
+        <v>18</v>
+      </c>
       <c r="M22" s="25">
         <v>133.18103583163801</v>
       </c>
@@ -1729,7 +1752,7 @@
       <c r="J26" s="24"/>
       <c r="K26" s="24"/>
       <c r="L26" s="24" t="s">
-        <v>83</v>
+        <v>18</v>
       </c>
       <c r="M26" s="24"/>
     </row>
@@ -1766,7 +1789,7 @@
       <c r="J27" s="24"/>
       <c r="K27" s="24"/>
       <c r="L27" s="24" t="s">
-        <v>83</v>
+        <v>18</v>
       </c>
       <c r="M27" s="24"/>
     </row>
@@ -1803,7 +1826,7 @@
       <c r="J28" s="24"/>
       <c r="K28" s="24"/>
       <c r="L28" s="24" t="s">
-        <v>83</v>
+        <v>18</v>
       </c>
       <c r="M28" s="24"/>
     </row>
@@ -1839,7 +1862,9 @@
       </c>
       <c r="J29" s="22"/>
       <c r="K29" s="22"/>
-      <c r="L29" s="22"/>
+      <c r="L29" s="22" t="s">
+        <v>18</v>
+      </c>
       <c r="M29" s="22"/>
     </row>
     <row r="30" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1874,7 +1899,9 @@
       </c>
       <c r="J30" s="24"/>
       <c r="K30" s="24"/>
-      <c r="L30" s="24"/>
+      <c r="L30" s="24" t="s">
+        <v>18</v>
+      </c>
       <c r="M30" s="24"/>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
@@ -1909,7 +1936,9 @@
       </c>
       <c r="J31" s="22"/>
       <c r="K31" s="22"/>
-      <c r="L31" s="22"/>
+      <c r="L31" s="22" t="s">
+        <v>18</v>
+      </c>
       <c r="M31" s="22"/>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
@@ -1944,7 +1973,9 @@
       </c>
       <c r="J32" s="24"/>
       <c r="K32" s="24"/>
-      <c r="L32" s="24"/>
+      <c r="L32" s="24" t="s">
+        <v>18</v>
+      </c>
       <c r="M32" s="24"/>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
@@ -1979,7 +2010,9 @@
       </c>
       <c r="J33" s="15"/>
       <c r="K33" s="15"/>
-      <c r="L33" s="15"/>
+      <c r="L33" s="15" t="s">
+        <v>18</v>
+      </c>
       <c r="M33" s="15"/>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
@@ -2014,7 +2047,9 @@
       </c>
       <c r="J34" s="15"/>
       <c r="K34" s="15"/>
-      <c r="L34" s="15"/>
+      <c r="L34" s="15" t="s">
+        <v>18</v>
+      </c>
       <c r="M34" s="15"/>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.25">
@@ -2049,7 +2084,9 @@
       </c>
       <c r="J35" s="15"/>
       <c r="K35" s="15"/>
-      <c r="L35" s="15"/>
+      <c r="L35" s="15" t="s">
+        <v>18</v>
+      </c>
       <c r="M35" s="15"/>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.25">
@@ -2084,7 +2121,9 @@
       </c>
       <c r="J36" s="15"/>
       <c r="K36" s="15"/>
-      <c r="L36" s="15"/>
+      <c r="L36" s="15" t="s">
+        <v>18</v>
+      </c>
       <c r="M36" s="15"/>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.25">
@@ -2119,7 +2158,9 @@
       </c>
       <c r="J37" s="12"/>
       <c r="K37" s="12"/>
-      <c r="L37" s="12"/>
+      <c r="L37" s="12" t="s">
+        <v>18</v>
+      </c>
       <c r="M37" s="12"/>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.25">
@@ -2154,7 +2195,9 @@
       </c>
       <c r="J38" s="12"/>
       <c r="K38" s="12"/>
-      <c r="L38" s="12"/>
+      <c r="L38" s="12" t="s">
+        <v>18</v>
+      </c>
       <c r="M38" s="12"/>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.25">
@@ -2189,7 +2232,9 @@
       </c>
       <c r="J39" s="12"/>
       <c r="K39" s="12"/>
-      <c r="L39" s="12"/>
+      <c r="L39" s="12" t="s">
+        <v>18</v>
+      </c>
       <c r="M39" s="12"/>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.25">
@@ -2224,7 +2269,9 @@
       </c>
       <c r="J40" s="12"/>
       <c r="K40" s="12"/>
-      <c r="L40" s="12"/>
+      <c r="L40" s="12" t="s">
+        <v>18</v>
+      </c>
       <c r="M40" s="12"/>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.25">
@@ -4471,7 +4518,9 @@
       </c>
       <c r="J97" s="2"/>
       <c r="K97" s="2"/>
-      <c r="L97" s="2"/>
+      <c r="L97" s="2" t="s">
+        <v>18</v>
+      </c>
       <c r="M97" s="2"/>
     </row>
     <row r="98" spans="1:13" x14ac:dyDescent="0.25">
@@ -4506,7 +4555,9 @@
       </c>
       <c r="J98" s="2"/>
       <c r="K98" s="2"/>
-      <c r="L98" s="2"/>
+      <c r="L98" s="2" t="s">
+        <v>18</v>
+      </c>
       <c r="M98" s="2"/>
     </row>
     <row r="99" spans="1:13" x14ac:dyDescent="0.25">
@@ -4541,7 +4592,9 @@
       </c>
       <c r="J99" s="2"/>
       <c r="K99" s="2"/>
-      <c r="L99" s="2"/>
+      <c r="L99" s="2" t="s">
+        <v>18</v>
+      </c>
       <c r="M99" s="2"/>
     </row>
     <row r="100" spans="1:13" x14ac:dyDescent="0.25">
@@ -4576,7 +4629,9 @@
       </c>
       <c r="J100" s="2"/>
       <c r="K100" s="2"/>
-      <c r="L100" s="2"/>
+      <c r="L100" s="2" t="s">
+        <v>18</v>
+      </c>
       <c r="M100" s="2"/>
     </row>
     <row r="101" spans="1:13" x14ac:dyDescent="0.25">
@@ -4611,7 +4666,9 @@
       </c>
       <c r="J101" s="2"/>
       <c r="K101" s="2"/>
-      <c r="L101" s="2"/>
+      <c r="L101" s="2" t="s">
+        <v>18</v>
+      </c>
       <c r="M101" s="2"/>
     </row>
     <row r="102" spans="1:13" x14ac:dyDescent="0.25">
@@ -4646,7 +4703,9 @@
       </c>
       <c r="J102" s="2"/>
       <c r="K102" s="2"/>
-      <c r="L102" s="2"/>
+      <c r="L102" s="2" t="s">
+        <v>18</v>
+      </c>
       <c r="M102" s="2"/>
     </row>
     <row r="103" spans="1:13" x14ac:dyDescent="0.25">
@@ -4681,7 +4740,9 @@
       </c>
       <c r="J103" s="2"/>
       <c r="K103" s="2"/>
-      <c r="L103" s="2"/>
+      <c r="L103" s="2" t="s">
+        <v>18</v>
+      </c>
       <c r="M103" s="2"/>
     </row>
     <row r="104" spans="1:13" x14ac:dyDescent="0.25">
@@ -4716,7 +4777,9 @@
       </c>
       <c r="J104" s="2"/>
       <c r="K104" s="2"/>
-      <c r="L104" s="2"/>
+      <c r="L104" s="2" t="s">
+        <v>18</v>
+      </c>
       <c r="M104" s="2"/>
     </row>
     <row r="105" spans="1:13" x14ac:dyDescent="0.25">
@@ -4751,7 +4814,9 @@
       </c>
       <c r="J105" s="2"/>
       <c r="K105" s="2"/>
-      <c r="L105" s="2"/>
+      <c r="L105" s="2" t="s">
+        <v>18</v>
+      </c>
       <c r="M105" s="2"/>
     </row>
     <row r="106" spans="1:13" x14ac:dyDescent="0.25">
@@ -4786,7 +4851,9 @@
       </c>
       <c r="J106" s="2"/>
       <c r="K106" s="2"/>
-      <c r="L106" s="2"/>
+      <c r="L106" s="2" t="s">
+        <v>18</v>
+      </c>
       <c r="M106" s="2"/>
     </row>
     <row r="107" spans="1:13" x14ac:dyDescent="0.25">
@@ -4821,7 +4888,9 @@
       </c>
       <c r="J107" s="18"/>
       <c r="K107" s="18"/>
-      <c r="L107" s="18"/>
+      <c r="L107" s="18" t="s">
+        <v>18</v>
+      </c>
       <c r="M107" s="17"/>
     </row>
     <row r="108" spans="1:13" x14ac:dyDescent="0.25">
@@ -4856,7 +4925,9 @@
       </c>
       <c r="J108" s="18"/>
       <c r="K108" s="18"/>
-      <c r="L108" s="18"/>
+      <c r="L108" s="18" t="s">
+        <v>18</v>
+      </c>
       <c r="M108" s="18"/>
     </row>
     <row r="109" spans="1:13" x14ac:dyDescent="0.25">
@@ -4891,7 +4962,9 @@
       </c>
       <c r="J109" s="18"/>
       <c r="K109" s="18"/>
-      <c r="L109" s="18"/>
+      <c r="L109" s="18" t="s">
+        <v>18</v>
+      </c>
       <c r="M109" s="18"/>
     </row>
     <row r="110" spans="1:13" x14ac:dyDescent="0.25">
@@ -4926,7 +4999,9 @@
       </c>
       <c r="J110" s="18"/>
       <c r="K110" s="18"/>
-      <c r="L110" s="18"/>
+      <c r="L110" s="18" t="s">
+        <v>18</v>
+      </c>
       <c r="M110" s="18"/>
     </row>
     <row r="111" spans="1:13" x14ac:dyDescent="0.25">
@@ -4961,7 +5036,9 @@
       </c>
       <c r="J111" s="18"/>
       <c r="K111" s="18"/>
-      <c r="L111" s="18"/>
+      <c r="L111" s="18" t="s">
+        <v>18</v>
+      </c>
       <c r="M111" s="18"/>
     </row>
     <row r="112" spans="1:13" x14ac:dyDescent="0.25">
@@ -4996,7 +5073,9 @@
       </c>
       <c r="J112" s="18"/>
       <c r="K112" s="18"/>
-      <c r="L112" s="18"/>
+      <c r="L112" s="18" t="s">
+        <v>18</v>
+      </c>
       <c r="M112" s="18"/>
     </row>
     <row r="113" spans="1:13" x14ac:dyDescent="0.25">
@@ -5031,7 +5110,9 @@
       </c>
       <c r="J113" s="18"/>
       <c r="K113" s="18"/>
-      <c r="L113" s="18"/>
+      <c r="L113" s="18" t="s">
+        <v>18</v>
+      </c>
       <c r="M113" s="18"/>
     </row>
     <row r="114" spans="1:13" x14ac:dyDescent="0.25">
@@ -5066,7 +5147,9 @@
       </c>
       <c r="J114" s="18"/>
       <c r="K114" s="18"/>
-      <c r="L114" s="18"/>
+      <c r="L114" s="18" t="s">
+        <v>18</v>
+      </c>
       <c r="M114" s="18"/>
     </row>
     <row r="115" spans="1:13" x14ac:dyDescent="0.25">
@@ -5101,7 +5184,9 @@
       </c>
       <c r="J115" s="18"/>
       <c r="K115" s="18"/>
-      <c r="L115" s="18"/>
+      <c r="L115" s="18" t="s">
+        <v>18</v>
+      </c>
       <c r="M115" s="18"/>
     </row>
     <row r="116" spans="1:13" x14ac:dyDescent="0.25">
@@ -5136,7 +5221,9 @@
       </c>
       <c r="J116" s="18"/>
       <c r="K116" s="18"/>
-      <c r="L116" s="18"/>
+      <c r="L116" s="18" t="s">
+        <v>18</v>
+      </c>
       <c r="M116" s="18"/>
     </row>
     <row r="117" spans="1:13" x14ac:dyDescent="0.25">
@@ -5171,7 +5258,9 @@
       </c>
       <c r="J117" s="18"/>
       <c r="K117" s="18"/>
-      <c r="L117" s="18"/>
+      <c r="L117" s="18" t="s">
+        <v>18</v>
+      </c>
       <c r="M117" s="18"/>
     </row>
     <row r="118" spans="1:13" x14ac:dyDescent="0.25">
@@ -5206,7 +5295,9 @@
       </c>
       <c r="J118" s="18"/>
       <c r="K118" s="18"/>
-      <c r="L118" s="18"/>
+      <c r="L118" s="18" t="s">
+        <v>18</v>
+      </c>
       <c r="M118" s="18"/>
     </row>
     <row r="119" spans="1:13" x14ac:dyDescent="0.25">
@@ -5241,7 +5332,9 @@
       </c>
       <c r="J119" s="18"/>
       <c r="K119" s="18"/>
-      <c r="L119" s="18"/>
+      <c r="L119" s="18" t="s">
+        <v>18</v>
+      </c>
       <c r="M119" s="18"/>
     </row>
     <row r="120" spans="1:13" x14ac:dyDescent="0.25">
@@ -5276,7 +5369,9 @@
       </c>
       <c r="J120" s="18"/>
       <c r="K120" s="18"/>
-      <c r="L120" s="18"/>
+      <c r="L120" s="18" t="s">
+        <v>18</v>
+      </c>
       <c r="M120" s="18"/>
     </row>
     <row r="121" spans="1:13" x14ac:dyDescent="0.25">
@@ -5311,7 +5406,9 @@
       </c>
       <c r="J121" s="18"/>
       <c r="K121" s="18"/>
-      <c r="L121" s="18"/>
+      <c r="L121" s="18" t="s">
+        <v>18</v>
+      </c>
       <c r="M121" s="18"/>
     </row>
     <row r="122" spans="1:13" x14ac:dyDescent="0.25">
@@ -5346,7 +5443,9 @@
       </c>
       <c r="J122" s="18"/>
       <c r="K122" s="18"/>
-      <c r="L122" s="18"/>
+      <c r="L122" s="18" t="s">
+        <v>18</v>
+      </c>
       <c r="M122" s="18"/>
     </row>
     <row r="123" spans="1:13" x14ac:dyDescent="0.25">
@@ -5381,7 +5480,9 @@
       </c>
       <c r="J123" s="20"/>
       <c r="K123" s="20"/>
-      <c r="L123" s="20"/>
+      <c r="L123" s="18" t="s">
+        <v>18</v>
+      </c>
       <c r="M123" s="20"/>
     </row>
     <row r="124" spans="1:13" x14ac:dyDescent="0.25">
@@ -5416,7 +5517,9 @@
       </c>
       <c r="J124" s="20"/>
       <c r="K124" s="20"/>
-      <c r="L124" s="20"/>
+      <c r="L124" s="18" t="s">
+        <v>18</v>
+      </c>
       <c r="M124" s="20"/>
     </row>
     <row r="125" spans="1:13" x14ac:dyDescent="0.25">
@@ -5451,7 +5554,9 @@
       </c>
       <c r="J125" s="20"/>
       <c r="K125" s="20"/>
-      <c r="L125" s="20"/>
+      <c r="L125" s="18" t="s">
+        <v>18</v>
+      </c>
       <c r="M125" s="20"/>
     </row>
     <row r="126" spans="1:13" x14ac:dyDescent="0.25">
@@ -5486,7 +5591,9 @@
       </c>
       <c r="J126" s="20"/>
       <c r="K126" s="20"/>
-      <c r="L126" s="20"/>
+      <c r="L126" s="18" t="s">
+        <v>18</v>
+      </c>
       <c r="M126" s="20"/>
     </row>
     <row r="127" spans="1:13" x14ac:dyDescent="0.25">
@@ -5521,7 +5628,9 @@
       </c>
       <c r="J127" s="20"/>
       <c r="K127" s="20"/>
-      <c r="L127" s="20"/>
+      <c r="L127" s="18" t="s">
+        <v>18</v>
+      </c>
       <c r="M127" s="20"/>
     </row>
     <row r="128" spans="1:13" x14ac:dyDescent="0.25">
@@ -5556,7 +5665,9 @@
       </c>
       <c r="J128" s="20"/>
       <c r="K128" s="20"/>
-      <c r="L128" s="20"/>
+      <c r="L128" s="18" t="s">
+        <v>18</v>
+      </c>
       <c r="M128" s="20"/>
     </row>
     <row r="129" spans="1:13" x14ac:dyDescent="0.25">
@@ -5591,7 +5702,9 @@
       </c>
       <c r="J129" s="20"/>
       <c r="K129" s="20"/>
-      <c r="L129" s="20"/>
+      <c r="L129" s="18" t="s">
+        <v>18</v>
+      </c>
       <c r="M129" s="20"/>
     </row>
     <row r="130" spans="1:13" x14ac:dyDescent="0.25">
@@ -5626,7 +5739,9 @@
       </c>
       <c r="J130" s="20"/>
       <c r="K130" s="20"/>
-      <c r="L130" s="20"/>
+      <c r="L130" s="18" t="s">
+        <v>18</v>
+      </c>
       <c r="M130" s="20"/>
     </row>
     <row r="131" spans="1:13" x14ac:dyDescent="0.25">
@@ -5661,7 +5776,9 @@
       </c>
       <c r="J131" s="20"/>
       <c r="K131" s="20"/>
-      <c r="L131" s="20"/>
+      <c r="L131" s="18" t="s">
+        <v>18</v>
+      </c>
       <c r="M131" s="20"/>
     </row>
     <row r="132" spans="1:13" x14ac:dyDescent="0.25">
@@ -5696,7 +5813,9 @@
       </c>
       <c r="J132" s="20"/>
       <c r="K132" s="20"/>
-      <c r="L132" s="20"/>
+      <c r="L132" s="18" t="s">
+        <v>18</v>
+      </c>
       <c r="M132" s="20"/>
     </row>
     <row r="133" spans="1:13" x14ac:dyDescent="0.25">
@@ -5731,7 +5850,9 @@
       </c>
       <c r="J133" s="20"/>
       <c r="K133" s="20"/>
-      <c r="L133" s="20"/>
+      <c r="L133" s="18" t="s">
+        <v>18</v>
+      </c>
       <c r="M133" s="20"/>
     </row>
     <row r="134" spans="1:13" x14ac:dyDescent="0.25">
@@ -5766,7 +5887,9 @@
       </c>
       <c r="J134" s="20"/>
       <c r="K134" s="20"/>
-      <c r="L134" s="20"/>
+      <c r="L134" s="18" t="s">
+        <v>18</v>
+      </c>
       <c r="M134" s="20"/>
     </row>
     <row r="135" spans="1:13" x14ac:dyDescent="0.25">
@@ -5801,7 +5924,9 @@
       </c>
       <c r="J135" s="20"/>
       <c r="K135" s="20"/>
-      <c r="L135" s="20"/>
+      <c r="L135" s="18" t="s">
+        <v>18</v>
+      </c>
       <c r="M135" s="20"/>
     </row>
     <row r="136" spans="1:13" x14ac:dyDescent="0.25">
@@ -5836,7 +5961,9 @@
       </c>
       <c r="J136" s="20"/>
       <c r="K136" s="20"/>
-      <c r="L136" s="20"/>
+      <c r="L136" s="18" t="s">
+        <v>18</v>
+      </c>
       <c r="M136" s="20"/>
     </row>
     <row r="137" spans="1:13" x14ac:dyDescent="0.25">
@@ -5871,7 +5998,9 @@
       </c>
       <c r="J137" s="20"/>
       <c r="K137" s="20"/>
-      <c r="L137" s="20"/>
+      <c r="L137" s="18" t="s">
+        <v>18</v>
+      </c>
       <c r="M137" s="20"/>
     </row>
     <row r="138" spans="1:13" x14ac:dyDescent="0.25">
@@ -5906,7 +6035,9 @@
       </c>
       <c r="J138" s="20"/>
       <c r="K138" s="20"/>
-      <c r="L138" s="20"/>
+      <c r="L138" s="18" t="s">
+        <v>18</v>
+      </c>
       <c r="M138" s="20"/>
     </row>
     <row r="139" spans="1:13" x14ac:dyDescent="0.25">
@@ -5941,7 +6072,9 @@
       </c>
       <c r="J139" s="18"/>
       <c r="K139" s="18"/>
-      <c r="L139" s="18"/>
+      <c r="L139" s="18" t="s">
+        <v>18</v>
+      </c>
       <c r="M139" s="18"/>
     </row>
     <row r="140" spans="1:13" x14ac:dyDescent="0.25">
@@ -5976,7 +6109,9 @@
       </c>
       <c r="J140" s="18"/>
       <c r="K140" s="18"/>
-      <c r="L140" s="18"/>
+      <c r="L140" s="18" t="s">
+        <v>18</v>
+      </c>
       <c r="M140" s="18"/>
     </row>
     <row r="141" spans="1:13" x14ac:dyDescent="0.25">
@@ -6011,7 +6146,9 @@
       </c>
       <c r="J141" s="18"/>
       <c r="K141" s="18"/>
-      <c r="L141" s="18"/>
+      <c r="L141" s="18" t="s">
+        <v>18</v>
+      </c>
       <c r="M141" s="18"/>
     </row>
     <row r="142" spans="1:13" x14ac:dyDescent="0.25">
@@ -6046,7 +6183,9 @@
       </c>
       <c r="J142" s="18"/>
       <c r="K142" s="18"/>
-      <c r="L142" s="18"/>
+      <c r="L142" s="18" t="s">
+        <v>18</v>
+      </c>
       <c r="M142" s="18"/>
     </row>
     <row r="143" spans="1:13" x14ac:dyDescent="0.25">
@@ -6081,7 +6220,9 @@
       </c>
       <c r="J143" s="18"/>
       <c r="K143" s="18"/>
-      <c r="L143" s="18"/>
+      <c r="L143" s="18" t="s">
+        <v>18</v>
+      </c>
       <c r="M143" s="18"/>
     </row>
     <row r="144" spans="1:13" x14ac:dyDescent="0.25">
@@ -6116,7 +6257,9 @@
       </c>
       <c r="J144" s="18"/>
       <c r="K144" s="18"/>
-      <c r="L144" s="18"/>
+      <c r="L144" s="18" t="s">
+        <v>18</v>
+      </c>
       <c r="M144" s="18"/>
     </row>
     <row r="145" spans="1:13" x14ac:dyDescent="0.25">
@@ -6151,7 +6294,9 @@
       </c>
       <c r="J145" s="18"/>
       <c r="K145" s="18"/>
-      <c r="L145" s="18"/>
+      <c r="L145" s="18" t="s">
+        <v>18</v>
+      </c>
       <c r="M145" s="18"/>
     </row>
     <row r="146" spans="1:13" x14ac:dyDescent="0.25">
@@ -6186,7 +6331,9 @@
       </c>
       <c r="J146" s="18"/>
       <c r="K146" s="18"/>
-      <c r="L146" s="18"/>
+      <c r="L146" s="18" t="s">
+        <v>18</v>
+      </c>
       <c r="M146" s="18"/>
     </row>
     <row r="147" spans="1:13" x14ac:dyDescent="0.25">
@@ -6221,7 +6368,9 @@
       </c>
       <c r="J147" s="18"/>
       <c r="K147" s="18"/>
-      <c r="L147" s="18"/>
+      <c r="L147" s="18" t="s">
+        <v>18</v>
+      </c>
       <c r="M147" s="18"/>
     </row>
     <row r="148" spans="1:13" x14ac:dyDescent="0.25">
@@ -6256,7 +6405,9 @@
       </c>
       <c r="J148" s="18"/>
       <c r="K148" s="18"/>
-      <c r="L148" s="18"/>
+      <c r="L148" s="18" t="s">
+        <v>18</v>
+      </c>
       <c r="M148" s="18"/>
     </row>
     <row r="149" spans="1:13" x14ac:dyDescent="0.25">
@@ -6291,7 +6442,9 @@
       </c>
       <c r="J149" s="18"/>
       <c r="K149" s="18"/>
-      <c r="L149" s="18"/>
+      <c r="L149" s="18" t="s">
+        <v>18</v>
+      </c>
       <c r="M149" s="18"/>
     </row>
     <row r="150" spans="1:13" x14ac:dyDescent="0.25">
@@ -6326,7 +6479,9 @@
       </c>
       <c r="J150" s="18"/>
       <c r="K150" s="18"/>
-      <c r="L150" s="18"/>
+      <c r="L150" s="18" t="s">
+        <v>18</v>
+      </c>
       <c r="M150" s="18"/>
     </row>
     <row r="151" spans="1:13" x14ac:dyDescent="0.25">
@@ -6361,7 +6516,9 @@
       </c>
       <c r="J151" s="18"/>
       <c r="K151" s="18"/>
-      <c r="L151" s="18"/>
+      <c r="L151" s="18" t="s">
+        <v>18</v>
+      </c>
       <c r="M151" s="18"/>
     </row>
     <row r="152" spans="1:13" x14ac:dyDescent="0.25">
@@ -6396,7 +6553,9 @@
       </c>
       <c r="J152" s="18"/>
       <c r="K152" s="18"/>
-      <c r="L152" s="18"/>
+      <c r="L152" s="18" t="s">
+        <v>18</v>
+      </c>
       <c r="M152" s="18"/>
     </row>
     <row r="153" spans="1:13" x14ac:dyDescent="0.25">
@@ -6431,7 +6590,9 @@
       </c>
       <c r="J153" s="18"/>
       <c r="K153" s="18"/>
-      <c r="L153" s="18"/>
+      <c r="L153" s="18" t="s">
+        <v>18</v>
+      </c>
       <c r="M153" s="18"/>
     </row>
     <row r="154" spans="1:13" x14ac:dyDescent="0.25">
@@ -6466,7 +6627,9 @@
       </c>
       <c r="J154" s="18"/>
       <c r="K154" s="18"/>
-      <c r="L154" s="18"/>
+      <c r="L154" s="18" t="s">
+        <v>18</v>
+      </c>
       <c r="M154" s="18"/>
     </row>
     <row r="155" spans="1:13" x14ac:dyDescent="0.25">
@@ -6501,7 +6664,9 @@
       </c>
       <c r="J155" s="20"/>
       <c r="K155" s="20"/>
-      <c r="L155" s="20"/>
+      <c r="L155" s="18" t="s">
+        <v>18</v>
+      </c>
       <c r="M155" s="20"/>
     </row>
     <row r="156" spans="1:13" x14ac:dyDescent="0.25">
@@ -6536,7 +6701,9 @@
       </c>
       <c r="J156" s="20"/>
       <c r="K156" s="20"/>
-      <c r="L156" s="20"/>
+      <c r="L156" s="18" t="s">
+        <v>18</v>
+      </c>
       <c r="M156" s="20"/>
     </row>
     <row r="157" spans="1:13" x14ac:dyDescent="0.25">
@@ -6571,7 +6738,9 @@
       </c>
       <c r="J157" s="20"/>
       <c r="K157" s="20"/>
-      <c r="L157" s="20"/>
+      <c r="L157" s="18" t="s">
+        <v>18</v>
+      </c>
       <c r="M157" s="20"/>
     </row>
     <row r="158" spans="1:13" x14ac:dyDescent="0.25">
@@ -6606,7 +6775,9 @@
       </c>
       <c r="J158" s="20"/>
       <c r="K158" s="20"/>
-      <c r="L158" s="20"/>
+      <c r="L158" s="18" t="s">
+        <v>18</v>
+      </c>
       <c r="M158" s="20"/>
     </row>
     <row r="159" spans="1:13" x14ac:dyDescent="0.25">
@@ -6641,7 +6812,9 @@
       </c>
       <c r="J159" s="20"/>
       <c r="K159" s="20"/>
-      <c r="L159" s="20"/>
+      <c r="L159" s="18" t="s">
+        <v>18</v>
+      </c>
       <c r="M159" s="20"/>
     </row>
     <row r="160" spans="1:13" x14ac:dyDescent="0.25">
@@ -6676,7 +6849,9 @@
       </c>
       <c r="J160" s="20"/>
       <c r="K160" s="20"/>
-      <c r="L160" s="20"/>
+      <c r="L160" s="18" t="s">
+        <v>18</v>
+      </c>
       <c r="M160" s="20"/>
     </row>
     <row r="161" spans="1:13" x14ac:dyDescent="0.25">
@@ -6711,7 +6886,9 @@
       </c>
       <c r="J161" s="20"/>
       <c r="K161" s="20"/>
-      <c r="L161" s="20"/>
+      <c r="L161" s="18" t="s">
+        <v>18</v>
+      </c>
       <c r="M161" s="20"/>
     </row>
     <row r="162" spans="1:13" x14ac:dyDescent="0.25">
@@ -6746,7 +6923,9 @@
       </c>
       <c r="J162" s="20"/>
       <c r="K162" s="20"/>
-      <c r="L162" s="20"/>
+      <c r="L162" s="18" t="s">
+        <v>18</v>
+      </c>
       <c r="M162" s="20"/>
     </row>
     <row r="163" spans="1:13" x14ac:dyDescent="0.25">
@@ -6781,7 +6960,9 @@
       </c>
       <c r="J163" s="20"/>
       <c r="K163" s="20"/>
-      <c r="L163" s="20"/>
+      <c r="L163" s="18" t="s">
+        <v>18</v>
+      </c>
       <c r="M163" s="20"/>
     </row>
     <row r="164" spans="1:13" x14ac:dyDescent="0.25">
@@ -6816,7 +6997,9 @@
       </c>
       <c r="J164" s="20"/>
       <c r="K164" s="20"/>
-      <c r="L164" s="20"/>
+      <c r="L164" s="18" t="s">
+        <v>18</v>
+      </c>
       <c r="M164" s="20"/>
     </row>
     <row r="165" spans="1:13" x14ac:dyDescent="0.25">
@@ -6851,7 +7034,9 @@
       </c>
       <c r="J165" s="20"/>
       <c r="K165" s="20"/>
-      <c r="L165" s="20"/>
+      <c r="L165" s="18" t="s">
+        <v>18</v>
+      </c>
       <c r="M165" s="20"/>
     </row>
     <row r="166" spans="1:13" x14ac:dyDescent="0.25">
@@ -6886,7 +7071,9 @@
       </c>
       <c r="J166" s="20"/>
       <c r="K166" s="20"/>
-      <c r="L166" s="20"/>
+      <c r="L166" s="18" t="s">
+        <v>18</v>
+      </c>
       <c r="M166" s="20"/>
     </row>
     <row r="167" spans="1:13" x14ac:dyDescent="0.25">
@@ -6921,7 +7108,9 @@
       </c>
       <c r="J167" s="20"/>
       <c r="K167" s="20"/>
-      <c r="L167" s="20"/>
+      <c r="L167" s="18" t="s">
+        <v>18</v>
+      </c>
       <c r="M167" s="20"/>
     </row>
     <row r="168" spans="1:13" x14ac:dyDescent="0.25">
@@ -6956,7 +7145,9 @@
       </c>
       <c r="J168" s="20"/>
       <c r="K168" s="20"/>
-      <c r="L168" s="20"/>
+      <c r="L168" s="18" t="s">
+        <v>18</v>
+      </c>
       <c r="M168" s="20"/>
     </row>
     <row r="169" spans="1:13" x14ac:dyDescent="0.25">
@@ -6991,7 +7182,9 @@
       </c>
       <c r="J169" s="20"/>
       <c r="K169" s="20"/>
-      <c r="L169" s="20"/>
+      <c r="L169" s="18" t="s">
+        <v>18</v>
+      </c>
       <c r="M169" s="20"/>
     </row>
     <row r="170" spans="1:13" x14ac:dyDescent="0.25">
@@ -7026,12 +7219,14 @@
       </c>
       <c r="J170" s="20"/>
       <c r="K170" s="20"/>
-      <c r="L170" s="20"/>
+      <c r="L170" s="18" t="s">
+        <v>18</v>
+      </c>
       <c r="M170" s="20"/>
     </row>
     <row r="171" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A171" s="18" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B171" s="18" t="s">
         <v>52</v>
@@ -7056,12 +7251,14 @@
       </c>
       <c r="J171" s="18"/>
       <c r="K171" s="18"/>
-      <c r="L171" s="18"/>
+      <c r="L171" s="18" t="s">
+        <v>18</v>
+      </c>
       <c r="M171" s="18"/>
     </row>
     <row r="172" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A172" s="18" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B172" s="18" t="s">
         <v>52</v>
@@ -7086,12 +7283,14 @@
       </c>
       <c r="J172" s="18"/>
       <c r="K172" s="18"/>
-      <c r="L172" s="18"/>
+      <c r="L172" s="18" t="s">
+        <v>18</v>
+      </c>
       <c r="M172" s="18"/>
     </row>
     <row r="173" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A173" s="18" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B173" s="18" t="s">
         <v>52</v>
@@ -7116,12 +7315,14 @@
       </c>
       <c r="J173" s="18"/>
       <c r="K173" s="18"/>
-      <c r="L173" s="18"/>
+      <c r="L173" s="18" t="s">
+        <v>18</v>
+      </c>
       <c r="M173" s="18"/>
     </row>
     <row r="174" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A174" s="18" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B174" s="18" t="s">
         <v>52</v>
@@ -7146,7 +7347,9 @@
       </c>
       <c r="J174" s="18"/>
       <c r="K174" s="18"/>
-      <c r="L174" s="18"/>
+      <c r="L174" s="18" t="s">
+        <v>18</v>
+      </c>
       <c r="M174" s="18"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update usage status for CIN1/2/3 prev data in Excel
</commit_message>
<xml_diff>
--- a/Config/Calibration_targets_Kenya.xlsx
+++ b/Config/Calibration_targets_Kenya.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\HHCoM\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89D5381A-B9E7-486E-9B3F-177201184EF2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC5D01F0-731F-4086-98A7-71E075F1AC0F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="870" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="870" uniqueCount="85">
   <si>
     <t>Criteria</t>
   </si>
@@ -277,6 +277,9 @@
   </si>
   <si>
     <t xml:space="preserve">Total population size </t>
+  </si>
+  <si>
+    <t>N</t>
   </si>
 </sst>
 </file>
@@ -803,13 +806,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M174"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A106" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F97" sqref="F97"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="L28" sqref="L28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.28515625" customWidth="1"/>
+    <col min="1" max="1" width="36" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23.42578125" customWidth="1"/>
     <col min="3" max="3" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
@@ -1752,7 +1755,7 @@
       <c r="J26" s="24"/>
       <c r="K26" s="24"/>
       <c r="L26" s="24" t="s">
-        <v>18</v>
+        <v>84</v>
       </c>
       <c r="M26" s="24"/>
     </row>
@@ -1789,7 +1792,7 @@
       <c r="J27" s="24"/>
       <c r="K27" s="24"/>
       <c r="L27" s="24" t="s">
-        <v>18</v>
+        <v>84</v>
       </c>
       <c r="M27" s="24"/>
     </row>
@@ -1826,7 +1829,7 @@
       <c r="J28" s="24"/>
       <c r="K28" s="24"/>
       <c r="L28" s="24" t="s">
-        <v>18</v>
+        <v>84</v>
       </c>
       <c r="M28" s="24"/>
     </row>

</xml_diff>

<commit_message>
Updated calibration targets to include KAIS 2012 HIV by sex
</commit_message>
<xml_diff>
--- a/Config/Calibration_targets_Kenya.xlsx
+++ b/Config/Calibration_targets_Kenya.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20363"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20364"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\udrive.uw.edu\udrive\Kenya_model_HPV-HIVacq\HHCoM\Config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Kenya_model_Feb20\HHCoM\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77FBC3E7-4A35-4B22-96AC-7AB4A3DFDF46}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0F7DA8E-CFBC-425C-8375-3E17C9E9B439}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9525" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Calibration" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="767" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1270" uniqueCount="91">
   <si>
     <t>Criteria</t>
   </si>
@@ -281,6 +281,24 @@
   <si>
     <t xml:space="preserve">Total population size </t>
   </si>
+  <si>
+    <t>HIV prevalence in men</t>
+  </si>
+  <si>
+    <t xml:space="preserve">All </t>
+  </si>
+  <si>
+    <t>HIV prevalence in men 2012</t>
+  </si>
+  <si>
+    <t>HIV prevalence in women 2012</t>
+  </si>
+  <si>
+    <t>UNAIDS 2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HIV prevalence in women </t>
+  </si>
 </sst>
 </file>
 
@@ -291,7 +309,7 @@
     <numFmt numFmtId="165" formatCode="0.000"/>
     <numFmt numFmtId="166" formatCode="0.000000000"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -306,8 +324,146 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="12">
+  <fills count="46">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -316,19 +472,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF1E8F8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFEFEF"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFD5D5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -374,8 +518,211 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEBEB"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCDCD"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF6F0FA"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFEADCF4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -398,84 +745,317 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="11">
+  <cellStyleXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="42" borderId="1" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="1" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="1" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="1" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="45" borderId="1" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="44" borderId="1" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="43" borderId="1" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="18" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="10">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="11">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="11">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="41" borderId="1" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="2" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="0" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="0" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="1" fontId="0" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="1" fontId="0" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="2" quotePrefix="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="3" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="3" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="42" borderId="1" xfId="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="42" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="42" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="42" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="42" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="2" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="3" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="3" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="3" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="4" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="5" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="4" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="5" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="5" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="6" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="5" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="6" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="6" applyFont="1"/>
-    <xf numFmtId="49" fontId="0" fillId="7" borderId="1" xfId="5" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="7" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="7" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="6" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="1" xfId="5" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="7" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="7" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="8" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="9" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="10" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="10" quotePrefix="1" applyFont="1"/>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="1" xfId="10" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="8" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="9" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="45" borderId="1" xfId="10" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="45" borderId="1" xfId="10" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="45" borderId="1" xfId="10" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="2" borderId="1" xfId="10" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="0" fillId="11" borderId="1" xfId="9" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="0" fillId="10" borderId="1" xfId="7" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="0" fillId="9" borderId="1" xfId="8" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="0" fillId="6" borderId="1" xfId="4" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="0" fillId="5" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="0" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="0" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="0" fillId="7" borderId="1" xfId="5" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="0" fillId="8" borderId="1" xfId="6" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="45" borderId="1" xfId="10" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="9" borderId="1" xfId="9" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="8" borderId="1" xfId="7" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="7" borderId="1" xfId="8" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="4" borderId="1" xfId="4" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="3" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="2" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="42" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="5" borderId="1" xfId="5" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="6" borderId="1" xfId="6" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="45" borderId="1" xfId="10" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="44" borderId="1" xfId="44" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="43" borderId="1" xfId="46" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="44" borderId="1" xfId="44" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="18" fillId="45" borderId="1" xfId="10" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="11">
+  <cellStyles count="64">
+    <cellStyle name="20% - Accent1" xfId="27" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="30" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="33" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="36" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="39" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="42" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="28" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="31" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="34" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="37" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="40" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="43" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1 2" xfId="47" xr:uid="{00000000-0005-0000-0000-000039000000}"/>
+    <cellStyle name="60% - Accent2 2" xfId="48" xr:uid="{00000000-0005-0000-0000-00003A000000}"/>
+    <cellStyle name="60% - Accent3 2" xfId="49" xr:uid="{00000000-0005-0000-0000-00003B000000}"/>
+    <cellStyle name="60% - Accent4 2" xfId="50" xr:uid="{00000000-0005-0000-0000-00003C000000}"/>
+    <cellStyle name="60% - Accent5 2" xfId="51" xr:uid="{00000000-0005-0000-0000-00003D000000}"/>
+    <cellStyle name="60% - Accent6 2" xfId="52" xr:uid="{00000000-0005-0000-0000-00003E000000}"/>
+    <cellStyle name="Accent1" xfId="26" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="29" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="32" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="35" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="38" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="41" builtinId="49" customBuiltin="1"/>
     <cellStyle name="Attrib" xfId="10" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="Attrib 2" xfId="44" xr:uid="{DA877E2D-0478-4338-B712-F45EC6BCE671}"/>
+    <cellStyle name="Bad" xfId="16" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="19" builtinId="22" customBuiltin="1"/>
     <cellStyle name="CC" xfId="9" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Check Cell" xfId="21" builtinId="23" customBuiltin="1"/>
     <cellStyle name="CIN" xfId="7" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
     <cellStyle name="CIN 2" xfId="8" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
-    <cellStyle name="HIVM" xfId="1" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="Data" xfId="57" xr:uid="{00000000-0005-0000-0000-00001D000000}"/>
+    <cellStyle name="Data 2" xfId="59" xr:uid="{00000000-0005-0000-0000-00001E000000}"/>
+    <cellStyle name="Explanatory Text" xfId="24" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="15" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Header" xfId="56" xr:uid="{00000000-0005-0000-0000-000021000000}"/>
+    <cellStyle name="Heading 1" xfId="11" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="12" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="13" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="14" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="HIVF" xfId="1" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="HIVM" xfId="46" xr:uid="{ADAFB709-FF9D-4146-8AE8-01B6B550B3ED}"/>
     <cellStyle name="HPV" xfId="3" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
     <cellStyle name="HPV 2" xfId="4" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="Input" xfId="17" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="20" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Neutral 2" xfId="45" xr:uid="{00000000-0005-0000-0000-000043000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="54" xr:uid="{00000000-0005-0000-0000-00002B000000}"/>
+    <cellStyle name="Normal 2 2" xfId="58" xr:uid="{00000000-0005-0000-0000-00002C000000}"/>
+    <cellStyle name="Note" xfId="23" builtinId="10" customBuiltin="1"/>
     <cellStyle name="Note 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
+    <cellStyle name="Note 2 2" xfId="61" xr:uid="{00000000-0005-0000-0000-00002E000000}"/>
+    <cellStyle name="Note 3" xfId="62" xr:uid="{00000000-0005-0000-0000-00002F000000}"/>
+    <cellStyle name="Note 4" xfId="63" xr:uid="{00000000-0005-0000-0000-000030000000}"/>
+    <cellStyle name="Output" xfId="18" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Percent 2" xfId="55" xr:uid="{00000000-0005-0000-0000-000033000000}"/>
     <cellStyle name="Population" xfId="5" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
     <cellStyle name="Population 2" xfId="6" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
+    <cellStyle name="Style 1" xfId="60" xr:uid="{00000000-0005-0000-0000-000034000000}"/>
+    <cellStyle name="Title 2" xfId="53" xr:uid="{00000000-0005-0000-0000-000035000000}"/>
+    <cellStyle name="Total" xfId="25" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="22" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="4">
     <dxf>
@@ -494,16 +1074,16 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFEADCF4"/>
+      <color rgb="FFF6F0FA"/>
+      <color rgb="FFFFCDCD"/>
+      <color rgb="FFFFEBEB"/>
       <color rgb="FFF1E8F8"/>
       <color rgb="FFFFEDB9"/>
       <color rgb="FFFFF7E1"/>
       <color rgb="FFC1EFFF"/>
       <color rgb="FFEBFAFF"/>
       <color rgb="FFFFD5D5"/>
-      <color rgb="FFFFEFEF"/>
-      <color rgb="FFFFBDBD"/>
-      <color rgb="FFFFDDDD"/>
-      <color rgb="FFEADCF4"/>
     </mruColors>
   </colors>
   <extLst>
@@ -518,8 +1098,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:M174" totalsRowShown="0">
-  <autoFilter ref="A1:M174" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:M254" totalsRowShown="0">
+  <autoFilter ref="A1:M254" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Criteria"/>
     <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Source"/>
@@ -804,10 +1384,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M174"/>
+  <dimension ref="A1:M254"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A96" sqref="A96"/>
+    <sheetView tabSelected="1" topLeftCell="A195" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="J225" sqref="J225"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1132,7 +1712,9 @@
       </c>
       <c r="J10" s="25"/>
       <c r="K10" s="25"/>
-      <c r="L10" s="25"/>
+      <c r="L10" s="25" t="s">
+        <v>18</v>
+      </c>
       <c r="M10" s="25">
         <f>Table1[[#This Row],[n]]/Table1[[#This Row],[Total N]]*100000</f>
         <v>0.71663276482550387</v>
@@ -1170,7 +1752,9 @@
       </c>
       <c r="J11" s="25"/>
       <c r="K11" s="25"/>
-      <c r="L11" s="25"/>
+      <c r="L11" s="25" t="s">
+        <v>18</v>
+      </c>
       <c r="M11" s="25">
         <v>0.84806759505553897</v>
       </c>
@@ -1207,7 +1791,9 @@
       </c>
       <c r="J12" s="25"/>
       <c r="K12" s="25"/>
-      <c r="L12" s="25"/>
+      <c r="L12" s="25" t="s">
+        <v>18</v>
+      </c>
       <c r="M12" s="25">
         <v>7.9909247379126498</v>
       </c>
@@ -1244,7 +1830,9 @@
       </c>
       <c r="J13" s="25"/>
       <c r="K13" s="25"/>
-      <c r="L13" s="25"/>
+      <c r="L13" s="25" t="s">
+        <v>18</v>
+      </c>
       <c r="M13" s="25">
         <v>20.976373024565699</v>
       </c>
@@ -1281,7 +1869,9 @@
       </c>
       <c r="J14" s="25"/>
       <c r="K14" s="25"/>
-      <c r="L14" s="25"/>
+      <c r="L14" s="25" t="s">
+        <v>18</v>
+      </c>
       <c r="M14" s="25">
         <v>40.716632764825398</v>
       </c>
@@ -1318,7 +1908,9 @@
       </c>
       <c r="J15" s="25"/>
       <c r="K15" s="25"/>
-      <c r="L15" s="25"/>
+      <c r="L15" s="25" t="s">
+        <v>18</v>
+      </c>
       <c r="M15" s="25">
         <v>62.664684712877403</v>
       </c>
@@ -1355,7 +1947,9 @@
       </c>
       <c r="J16" s="25"/>
       <c r="K16" s="25"/>
-      <c r="L16" s="25"/>
+      <c r="L16" s="25" t="s">
+        <v>18</v>
+      </c>
       <c r="M16" s="25">
         <v>83.052730402127906</v>
       </c>
@@ -1392,7 +1986,9 @@
       </c>
       <c r="J17" s="25"/>
       <c r="K17" s="25"/>
-      <c r="L17" s="25"/>
+      <c r="L17" s="25" t="s">
+        <v>18</v>
+      </c>
       <c r="M17" s="25">
         <v>103.442340791738</v>
       </c>
@@ -1429,7 +2025,9 @@
       </c>
       <c r="J18" s="25"/>
       <c r="K18" s="25"/>
-      <c r="L18" s="25"/>
+      <c r="L18" s="25" t="s">
+        <v>18</v>
+      </c>
       <c r="M18" s="25">
         <v>130.32389297449501</v>
       </c>
@@ -1466,7 +2064,9 @@
       </c>
       <c r="J19" s="25"/>
       <c r="K19" s="25"/>
-      <c r="L19" s="25"/>
+      <c r="L19" s="25" t="s">
+        <v>18</v>
+      </c>
       <c r="M19" s="25">
         <v>150.45376310436501</v>
       </c>
@@ -1503,7 +2103,9 @@
       </c>
       <c r="J20" s="25"/>
       <c r="K20" s="25"/>
-      <c r="L20" s="25"/>
+      <c r="L20" s="25" t="s">
+        <v>18</v>
+      </c>
       <c r="M20" s="25">
         <v>156.29791894852099</v>
       </c>
@@ -1540,7 +2142,9 @@
       </c>
       <c r="J21" s="25"/>
       <c r="K21" s="25"/>
-      <c r="L21" s="25"/>
+      <c r="L21" s="25" t="s">
+        <v>18</v>
+      </c>
       <c r="M21" s="25">
         <v>150.71350336410501</v>
       </c>
@@ -1577,7 +2181,9 @@
       </c>
       <c r="J22" s="25"/>
       <c r="K22" s="25"/>
-      <c r="L22" s="25"/>
+      <c r="L22" s="25" t="s">
+        <v>18</v>
+      </c>
       <c r="M22" s="25">
         <v>133.18103583163801</v>
       </c>
@@ -1839,7 +2445,9 @@
       </c>
       <c r="J29" s="22"/>
       <c r="K29" s="22"/>
-      <c r="L29" s="22"/>
+      <c r="L29" s="22" t="s">
+        <v>18</v>
+      </c>
       <c r="M29" s="22"/>
     </row>
     <row r="30" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1874,7 +2482,9 @@
       </c>
       <c r="J30" s="24"/>
       <c r="K30" s="24"/>
-      <c r="L30" s="24"/>
+      <c r="L30" s="24" t="s">
+        <v>18</v>
+      </c>
       <c r="M30" s="24"/>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
@@ -1909,7 +2519,9 @@
       </c>
       <c r="J31" s="22"/>
       <c r="K31" s="22"/>
-      <c r="L31" s="22"/>
+      <c r="L31" s="22" t="s">
+        <v>18</v>
+      </c>
       <c r="M31" s="22"/>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
@@ -1944,7 +2556,9 @@
       </c>
       <c r="J32" s="24"/>
       <c r="K32" s="24"/>
-      <c r="L32" s="24"/>
+      <c r="L32" s="24" t="s">
+        <v>18</v>
+      </c>
       <c r="M32" s="24"/>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
@@ -1979,7 +2593,9 @@
       </c>
       <c r="J33" s="15"/>
       <c r="K33" s="15"/>
-      <c r="L33" s="15"/>
+      <c r="L33" s="15" t="s">
+        <v>18</v>
+      </c>
       <c r="M33" s="15"/>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
@@ -2014,7 +2630,9 @@
       </c>
       <c r="J34" s="15"/>
       <c r="K34" s="15"/>
-      <c r="L34" s="15"/>
+      <c r="L34" s="15" t="s">
+        <v>18</v>
+      </c>
       <c r="M34" s="15"/>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.25">
@@ -2049,7 +2667,9 @@
       </c>
       <c r="J35" s="15"/>
       <c r="K35" s="15"/>
-      <c r="L35" s="15"/>
+      <c r="L35" s="15" t="s">
+        <v>18</v>
+      </c>
       <c r="M35" s="15"/>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.25">
@@ -2084,7 +2704,9 @@
       </c>
       <c r="J36" s="15"/>
       <c r="K36" s="15"/>
-      <c r="L36" s="15"/>
+      <c r="L36" s="15" t="s">
+        <v>18</v>
+      </c>
       <c r="M36" s="15"/>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.25">
@@ -2119,7 +2741,9 @@
       </c>
       <c r="J37" s="12"/>
       <c r="K37" s="12"/>
-      <c r="L37" s="12"/>
+      <c r="L37" s="12" t="s">
+        <v>18</v>
+      </c>
       <c r="M37" s="12"/>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.25">
@@ -2154,7 +2778,9 @@
       </c>
       <c r="J38" s="12"/>
       <c r="K38" s="12"/>
-      <c r="L38" s="12"/>
+      <c r="L38" s="12" t="s">
+        <v>18</v>
+      </c>
       <c r="M38" s="12"/>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.25">
@@ -2189,7 +2815,9 @@
       </c>
       <c r="J39" s="12"/>
       <c r="K39" s="12"/>
-      <c r="L39" s="12"/>
+      <c r="L39" s="12" t="s">
+        <v>18</v>
+      </c>
       <c r="M39" s="12"/>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.25">
@@ -2224,7 +2852,9 @@
       </c>
       <c r="J40" s="12"/>
       <c r="K40" s="12"/>
-      <c r="L40" s="12"/>
+      <c r="L40" s="12" t="s">
+        <v>18</v>
+      </c>
       <c r="M40" s="12"/>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.25">
@@ -4471,7 +5101,9 @@
       </c>
       <c r="J97" s="2"/>
       <c r="K97" s="2"/>
-      <c r="L97" s="2"/>
+      <c r="L97" s="3" t="s">
+        <v>18</v>
+      </c>
       <c r="M97" s="2"/>
     </row>
     <row r="98" spans="1:13" x14ac:dyDescent="0.25">
@@ -4506,7 +5138,9 @@
       </c>
       <c r="J98" s="2"/>
       <c r="K98" s="2"/>
-      <c r="L98" s="2"/>
+      <c r="L98" s="3" t="s">
+        <v>18</v>
+      </c>
       <c r="M98" s="2"/>
     </row>
     <row r="99" spans="1:13" x14ac:dyDescent="0.25">
@@ -4541,7 +5175,9 @@
       </c>
       <c r="J99" s="2"/>
       <c r="K99" s="2"/>
-      <c r="L99" s="2"/>
+      <c r="L99" s="3" t="s">
+        <v>18</v>
+      </c>
       <c r="M99" s="2"/>
     </row>
     <row r="100" spans="1:13" x14ac:dyDescent="0.25">
@@ -4576,7 +5212,9 @@
       </c>
       <c r="J100" s="2"/>
       <c r="K100" s="2"/>
-      <c r="L100" s="2"/>
+      <c r="L100" s="3" t="s">
+        <v>18</v>
+      </c>
       <c r="M100" s="2"/>
     </row>
     <row r="101" spans="1:13" x14ac:dyDescent="0.25">
@@ -4611,7 +5249,9 @@
       </c>
       <c r="J101" s="2"/>
       <c r="K101" s="2"/>
-      <c r="L101" s="2"/>
+      <c r="L101" s="3" t="s">
+        <v>18</v>
+      </c>
       <c r="M101" s="2"/>
     </row>
     <row r="102" spans="1:13" x14ac:dyDescent="0.25">
@@ -4646,7 +5286,9 @@
       </c>
       <c r="J102" s="2"/>
       <c r="K102" s="2"/>
-      <c r="L102" s="2"/>
+      <c r="L102" s="3" t="s">
+        <v>18</v>
+      </c>
       <c r="M102" s="2"/>
     </row>
     <row r="103" spans="1:13" x14ac:dyDescent="0.25">
@@ -4681,7 +5323,9 @@
       </c>
       <c r="J103" s="2"/>
       <c r="K103" s="2"/>
-      <c r="L103" s="2"/>
+      <c r="L103" s="3" t="s">
+        <v>18</v>
+      </c>
       <c r="M103" s="2"/>
     </row>
     <row r="104" spans="1:13" x14ac:dyDescent="0.25">
@@ -4716,7 +5360,9 @@
       </c>
       <c r="J104" s="2"/>
       <c r="K104" s="2"/>
-      <c r="L104" s="2"/>
+      <c r="L104" s="3" t="s">
+        <v>18</v>
+      </c>
       <c r="M104" s="2"/>
     </row>
     <row r="105" spans="1:13" x14ac:dyDescent="0.25">
@@ -4751,7 +5397,9 @@
       </c>
       <c r="J105" s="2"/>
       <c r="K105" s="2"/>
-      <c r="L105" s="2"/>
+      <c r="L105" s="3" t="s">
+        <v>18</v>
+      </c>
       <c r="M105" s="2"/>
     </row>
     <row r="106" spans="1:13" x14ac:dyDescent="0.25">
@@ -4786,7 +5434,9 @@
       </c>
       <c r="J106" s="2"/>
       <c r="K106" s="2"/>
-      <c r="L106" s="2"/>
+      <c r="L106" s="3" t="s">
+        <v>18</v>
+      </c>
       <c r="M106" s="2"/>
     </row>
     <row r="107" spans="1:13" x14ac:dyDescent="0.25">
@@ -4821,7 +5471,9 @@
       </c>
       <c r="J107" s="18"/>
       <c r="K107" s="18"/>
-      <c r="L107" s="18"/>
+      <c r="L107" s="18" t="s">
+        <v>18</v>
+      </c>
       <c r="M107" s="17"/>
     </row>
     <row r="108" spans="1:13" x14ac:dyDescent="0.25">
@@ -4856,7 +5508,9 @@
       </c>
       <c r="J108" s="18"/>
       <c r="K108" s="18"/>
-      <c r="L108" s="18"/>
+      <c r="L108" s="18" t="s">
+        <v>18</v>
+      </c>
       <c r="M108" s="18"/>
     </row>
     <row r="109" spans="1:13" x14ac:dyDescent="0.25">
@@ -4891,7 +5545,9 @@
       </c>
       <c r="J109" s="18"/>
       <c r="K109" s="18"/>
-      <c r="L109" s="18"/>
+      <c r="L109" s="18" t="s">
+        <v>18</v>
+      </c>
       <c r="M109" s="18"/>
     </row>
     <row r="110" spans="1:13" x14ac:dyDescent="0.25">
@@ -4926,7 +5582,9 @@
       </c>
       <c r="J110" s="18"/>
       <c r="K110" s="18"/>
-      <c r="L110" s="18"/>
+      <c r="L110" s="18" t="s">
+        <v>18</v>
+      </c>
       <c r="M110" s="18"/>
     </row>
     <row r="111" spans="1:13" x14ac:dyDescent="0.25">
@@ -4961,7 +5619,9 @@
       </c>
       <c r="J111" s="18"/>
       <c r="K111" s="18"/>
-      <c r="L111" s="18"/>
+      <c r="L111" s="18" t="s">
+        <v>18</v>
+      </c>
       <c r="M111" s="18"/>
     </row>
     <row r="112" spans="1:13" x14ac:dyDescent="0.25">
@@ -4996,7 +5656,9 @@
       </c>
       <c r="J112" s="18"/>
       <c r="K112" s="18"/>
-      <c r="L112" s="18"/>
+      <c r="L112" s="18" t="s">
+        <v>18</v>
+      </c>
       <c r="M112" s="18"/>
     </row>
     <row r="113" spans="1:13" x14ac:dyDescent="0.25">
@@ -5031,7 +5693,9 @@
       </c>
       <c r="J113" s="18"/>
       <c r="K113" s="18"/>
-      <c r="L113" s="18"/>
+      <c r="L113" s="18" t="s">
+        <v>18</v>
+      </c>
       <c r="M113" s="18"/>
     </row>
     <row r="114" spans="1:13" x14ac:dyDescent="0.25">
@@ -5066,7 +5730,9 @@
       </c>
       <c r="J114" s="18"/>
       <c r="K114" s="18"/>
-      <c r="L114" s="18"/>
+      <c r="L114" s="18" t="s">
+        <v>18</v>
+      </c>
       <c r="M114" s="18"/>
     </row>
     <row r="115" spans="1:13" x14ac:dyDescent="0.25">
@@ -5101,7 +5767,9 @@
       </c>
       <c r="J115" s="18"/>
       <c r="K115" s="18"/>
-      <c r="L115" s="18"/>
+      <c r="L115" s="18" t="s">
+        <v>18</v>
+      </c>
       <c r="M115" s="18"/>
     </row>
     <row r="116" spans="1:13" x14ac:dyDescent="0.25">
@@ -5136,7 +5804,9 @@
       </c>
       <c r="J116" s="18"/>
       <c r="K116" s="18"/>
-      <c r="L116" s="18"/>
+      <c r="L116" s="18" t="s">
+        <v>18</v>
+      </c>
       <c r="M116" s="18"/>
     </row>
     <row r="117" spans="1:13" x14ac:dyDescent="0.25">
@@ -5171,7 +5841,9 @@
       </c>
       <c r="J117" s="18"/>
       <c r="K117" s="18"/>
-      <c r="L117" s="18"/>
+      <c r="L117" s="18" t="s">
+        <v>18</v>
+      </c>
       <c r="M117" s="18"/>
     </row>
     <row r="118" spans="1:13" x14ac:dyDescent="0.25">
@@ -5206,7 +5878,9 @@
       </c>
       <c r="J118" s="18"/>
       <c r="K118" s="18"/>
-      <c r="L118" s="18"/>
+      <c r="L118" s="18" t="s">
+        <v>18</v>
+      </c>
       <c r="M118" s="18"/>
     </row>
     <row r="119" spans="1:13" x14ac:dyDescent="0.25">
@@ -5241,7 +5915,9 @@
       </c>
       <c r="J119" s="18"/>
       <c r="K119" s="18"/>
-      <c r="L119" s="18"/>
+      <c r="L119" s="18" t="s">
+        <v>18</v>
+      </c>
       <c r="M119" s="18"/>
     </row>
     <row r="120" spans="1:13" x14ac:dyDescent="0.25">
@@ -5276,7 +5952,9 @@
       </c>
       <c r="J120" s="18"/>
       <c r="K120" s="18"/>
-      <c r="L120" s="18"/>
+      <c r="L120" s="18" t="s">
+        <v>18</v>
+      </c>
       <c r="M120" s="18"/>
     </row>
     <row r="121" spans="1:13" x14ac:dyDescent="0.25">
@@ -5311,7 +5989,9 @@
       </c>
       <c r="J121" s="18"/>
       <c r="K121" s="18"/>
-      <c r="L121" s="18"/>
+      <c r="L121" s="18" t="s">
+        <v>18</v>
+      </c>
       <c r="M121" s="18"/>
     </row>
     <row r="122" spans="1:13" x14ac:dyDescent="0.25">
@@ -5346,7 +6026,9 @@
       </c>
       <c r="J122" s="18"/>
       <c r="K122" s="18"/>
-      <c r="L122" s="18"/>
+      <c r="L122" s="18" t="s">
+        <v>18</v>
+      </c>
       <c r="M122" s="18"/>
     </row>
     <row r="123" spans="1:13" x14ac:dyDescent="0.25">
@@ -5381,7 +6063,9 @@
       </c>
       <c r="J123" s="20"/>
       <c r="K123" s="20"/>
-      <c r="L123" s="20"/>
+      <c r="L123" s="20" t="s">
+        <v>18</v>
+      </c>
       <c r="M123" s="20"/>
     </row>
     <row r="124" spans="1:13" x14ac:dyDescent="0.25">
@@ -5416,7 +6100,9 @@
       </c>
       <c r="J124" s="20"/>
       <c r="K124" s="20"/>
-      <c r="L124" s="20"/>
+      <c r="L124" s="20" t="s">
+        <v>18</v>
+      </c>
       <c r="M124" s="20"/>
     </row>
     <row r="125" spans="1:13" x14ac:dyDescent="0.25">
@@ -5451,7 +6137,9 @@
       </c>
       <c r="J125" s="20"/>
       <c r="K125" s="20"/>
-      <c r="L125" s="20"/>
+      <c r="L125" s="20" t="s">
+        <v>18</v>
+      </c>
       <c r="M125" s="20"/>
     </row>
     <row r="126" spans="1:13" x14ac:dyDescent="0.25">
@@ -5486,7 +6174,9 @@
       </c>
       <c r="J126" s="20"/>
       <c r="K126" s="20"/>
-      <c r="L126" s="20"/>
+      <c r="L126" s="20" t="s">
+        <v>18</v>
+      </c>
       <c r="M126" s="20"/>
     </row>
     <row r="127" spans="1:13" x14ac:dyDescent="0.25">
@@ -5521,7 +6211,9 @@
       </c>
       <c r="J127" s="20"/>
       <c r="K127" s="20"/>
-      <c r="L127" s="20"/>
+      <c r="L127" s="20" t="s">
+        <v>18</v>
+      </c>
       <c r="M127" s="20"/>
     </row>
     <row r="128" spans="1:13" x14ac:dyDescent="0.25">
@@ -5556,7 +6248,9 @@
       </c>
       <c r="J128" s="20"/>
       <c r="K128" s="20"/>
-      <c r="L128" s="20"/>
+      <c r="L128" s="20" t="s">
+        <v>18</v>
+      </c>
       <c r="M128" s="20"/>
     </row>
     <row r="129" spans="1:13" x14ac:dyDescent="0.25">
@@ -5591,7 +6285,9 @@
       </c>
       <c r="J129" s="20"/>
       <c r="K129" s="20"/>
-      <c r="L129" s="20"/>
+      <c r="L129" s="20" t="s">
+        <v>18</v>
+      </c>
       <c r="M129" s="20"/>
     </row>
     <row r="130" spans="1:13" x14ac:dyDescent="0.25">
@@ -5626,7 +6322,9 @@
       </c>
       <c r="J130" s="20"/>
       <c r="K130" s="20"/>
-      <c r="L130" s="20"/>
+      <c r="L130" s="20" t="s">
+        <v>18</v>
+      </c>
       <c r="M130" s="20"/>
     </row>
     <row r="131" spans="1:13" x14ac:dyDescent="0.25">
@@ -5661,7 +6359,9 @@
       </c>
       <c r="J131" s="20"/>
       <c r="K131" s="20"/>
-      <c r="L131" s="20"/>
+      <c r="L131" s="20" t="s">
+        <v>18</v>
+      </c>
       <c r="M131" s="20"/>
     </row>
     <row r="132" spans="1:13" x14ac:dyDescent="0.25">
@@ -5696,7 +6396,9 @@
       </c>
       <c r="J132" s="20"/>
       <c r="K132" s="20"/>
-      <c r="L132" s="20"/>
+      <c r="L132" s="20" t="s">
+        <v>18</v>
+      </c>
       <c r="M132" s="20"/>
     </row>
     <row r="133" spans="1:13" x14ac:dyDescent="0.25">
@@ -5731,7 +6433,9 @@
       </c>
       <c r="J133" s="20"/>
       <c r="K133" s="20"/>
-      <c r="L133" s="20"/>
+      <c r="L133" s="20" t="s">
+        <v>18</v>
+      </c>
       <c r="M133" s="20"/>
     </row>
     <row r="134" spans="1:13" x14ac:dyDescent="0.25">
@@ -5766,7 +6470,9 @@
       </c>
       <c r="J134" s="20"/>
       <c r="K134" s="20"/>
-      <c r="L134" s="20"/>
+      <c r="L134" s="20" t="s">
+        <v>18</v>
+      </c>
       <c r="M134" s="20"/>
     </row>
     <row r="135" spans="1:13" x14ac:dyDescent="0.25">
@@ -5801,7 +6507,9 @@
       </c>
       <c r="J135" s="20"/>
       <c r="K135" s="20"/>
-      <c r="L135" s="20"/>
+      <c r="L135" s="20" t="s">
+        <v>18</v>
+      </c>
       <c r="M135" s="20"/>
     </row>
     <row r="136" spans="1:13" x14ac:dyDescent="0.25">
@@ -5836,7 +6544,9 @@
       </c>
       <c r="J136" s="20"/>
       <c r="K136" s="20"/>
-      <c r="L136" s="20"/>
+      <c r="L136" s="20" t="s">
+        <v>18</v>
+      </c>
       <c r="M136" s="20"/>
     </row>
     <row r="137" spans="1:13" x14ac:dyDescent="0.25">
@@ -5871,7 +6581,9 @@
       </c>
       <c r="J137" s="20"/>
       <c r="K137" s="20"/>
-      <c r="L137" s="20"/>
+      <c r="L137" s="20" t="s">
+        <v>18</v>
+      </c>
       <c r="M137" s="20"/>
     </row>
     <row r="138" spans="1:13" x14ac:dyDescent="0.25">
@@ -5906,7 +6618,9 @@
       </c>
       <c r="J138" s="20"/>
       <c r="K138" s="20"/>
-      <c r="L138" s="20"/>
+      <c r="L138" s="20" t="s">
+        <v>18</v>
+      </c>
       <c r="M138" s="20"/>
     </row>
     <row r="139" spans="1:13" x14ac:dyDescent="0.25">
@@ -5941,7 +6655,9 @@
       </c>
       <c r="J139" s="18"/>
       <c r="K139" s="18"/>
-      <c r="L139" s="18"/>
+      <c r="L139" s="18" t="s">
+        <v>18</v>
+      </c>
       <c r="M139" s="18"/>
     </row>
     <row r="140" spans="1:13" x14ac:dyDescent="0.25">
@@ -5976,7 +6692,9 @@
       </c>
       <c r="J140" s="18"/>
       <c r="K140" s="18"/>
-      <c r="L140" s="18"/>
+      <c r="L140" s="18" t="s">
+        <v>18</v>
+      </c>
       <c r="M140" s="18"/>
     </row>
     <row r="141" spans="1:13" x14ac:dyDescent="0.25">
@@ -6011,7 +6729,9 @@
       </c>
       <c r="J141" s="18"/>
       <c r="K141" s="18"/>
-      <c r="L141" s="18"/>
+      <c r="L141" s="18" t="s">
+        <v>18</v>
+      </c>
       <c r="M141" s="18"/>
     </row>
     <row r="142" spans="1:13" x14ac:dyDescent="0.25">
@@ -6046,7 +6766,9 @@
       </c>
       <c r="J142" s="18"/>
       <c r="K142" s="18"/>
-      <c r="L142" s="18"/>
+      <c r="L142" s="18" t="s">
+        <v>18</v>
+      </c>
       <c r="M142" s="18"/>
     </row>
     <row r="143" spans="1:13" x14ac:dyDescent="0.25">
@@ -6081,7 +6803,9 @@
       </c>
       <c r="J143" s="18"/>
       <c r="K143" s="18"/>
-      <c r="L143" s="18"/>
+      <c r="L143" s="18" t="s">
+        <v>18</v>
+      </c>
       <c r="M143" s="18"/>
     </row>
     <row r="144" spans="1:13" x14ac:dyDescent="0.25">
@@ -6116,7 +6840,9 @@
       </c>
       <c r="J144" s="18"/>
       <c r="K144" s="18"/>
-      <c r="L144" s="18"/>
+      <c r="L144" s="18" t="s">
+        <v>18</v>
+      </c>
       <c r="M144" s="18"/>
     </row>
     <row r="145" spans="1:13" x14ac:dyDescent="0.25">
@@ -6151,7 +6877,9 @@
       </c>
       <c r="J145" s="18"/>
       <c r="K145" s="18"/>
-      <c r="L145" s="18"/>
+      <c r="L145" s="18" t="s">
+        <v>18</v>
+      </c>
       <c r="M145" s="18"/>
     </row>
     <row r="146" spans="1:13" x14ac:dyDescent="0.25">
@@ -6186,7 +6914,9 @@
       </c>
       <c r="J146" s="18"/>
       <c r="K146" s="18"/>
-      <c r="L146" s="18"/>
+      <c r="L146" s="18" t="s">
+        <v>18</v>
+      </c>
       <c r="M146" s="18"/>
     </row>
     <row r="147" spans="1:13" x14ac:dyDescent="0.25">
@@ -6221,7 +6951,9 @@
       </c>
       <c r="J147" s="18"/>
       <c r="K147" s="18"/>
-      <c r="L147" s="18"/>
+      <c r="L147" s="18" t="s">
+        <v>18</v>
+      </c>
       <c r="M147" s="18"/>
     </row>
     <row r="148" spans="1:13" x14ac:dyDescent="0.25">
@@ -6256,7 +6988,9 @@
       </c>
       <c r="J148" s="18"/>
       <c r="K148" s="18"/>
-      <c r="L148" s="18"/>
+      <c r="L148" s="18" t="s">
+        <v>18</v>
+      </c>
       <c r="M148" s="18"/>
     </row>
     <row r="149" spans="1:13" x14ac:dyDescent="0.25">
@@ -6291,7 +7025,9 @@
       </c>
       <c r="J149" s="18"/>
       <c r="K149" s="18"/>
-      <c r="L149" s="18"/>
+      <c r="L149" s="18" t="s">
+        <v>18</v>
+      </c>
       <c r="M149" s="18"/>
     </row>
     <row r="150" spans="1:13" x14ac:dyDescent="0.25">
@@ -6326,7 +7062,9 @@
       </c>
       <c r="J150" s="18"/>
       <c r="K150" s="18"/>
-      <c r="L150" s="18"/>
+      <c r="L150" s="18" t="s">
+        <v>18</v>
+      </c>
       <c r="M150" s="18"/>
     </row>
     <row r="151" spans="1:13" x14ac:dyDescent="0.25">
@@ -6361,7 +7099,9 @@
       </c>
       <c r="J151" s="18"/>
       <c r="K151" s="18"/>
-      <c r="L151" s="18"/>
+      <c r="L151" s="18" t="s">
+        <v>18</v>
+      </c>
       <c r="M151" s="18"/>
     </row>
     <row r="152" spans="1:13" x14ac:dyDescent="0.25">
@@ -6396,7 +7136,9 @@
       </c>
       <c r="J152" s="18"/>
       <c r="K152" s="18"/>
-      <c r="L152" s="18"/>
+      <c r="L152" s="18" t="s">
+        <v>18</v>
+      </c>
       <c r="M152" s="18"/>
     </row>
     <row r="153" spans="1:13" x14ac:dyDescent="0.25">
@@ -6431,7 +7173,9 @@
       </c>
       <c r="J153" s="18"/>
       <c r="K153" s="18"/>
-      <c r="L153" s="18"/>
+      <c r="L153" s="18" t="s">
+        <v>18</v>
+      </c>
       <c r="M153" s="18"/>
     </row>
     <row r="154" spans="1:13" x14ac:dyDescent="0.25">
@@ -6466,7 +7210,9 @@
       </c>
       <c r="J154" s="18"/>
       <c r="K154" s="18"/>
-      <c r="L154" s="18"/>
+      <c r="L154" s="18" t="s">
+        <v>18</v>
+      </c>
       <c r="M154" s="18"/>
     </row>
     <row r="155" spans="1:13" x14ac:dyDescent="0.25">
@@ -6501,7 +7247,9 @@
       </c>
       <c r="J155" s="20"/>
       <c r="K155" s="20"/>
-      <c r="L155" s="20"/>
+      <c r="L155" s="20" t="s">
+        <v>18</v>
+      </c>
       <c r="M155" s="20"/>
     </row>
     <row r="156" spans="1:13" x14ac:dyDescent="0.25">
@@ -6536,7 +7284,9 @@
       </c>
       <c r="J156" s="20"/>
       <c r="K156" s="20"/>
-      <c r="L156" s="20"/>
+      <c r="L156" s="20" t="s">
+        <v>18</v>
+      </c>
       <c r="M156" s="20"/>
     </row>
     <row r="157" spans="1:13" x14ac:dyDescent="0.25">
@@ -6571,7 +7321,9 @@
       </c>
       <c r="J157" s="20"/>
       <c r="K157" s="20"/>
-      <c r="L157" s="20"/>
+      <c r="L157" s="20" t="s">
+        <v>18</v>
+      </c>
       <c r="M157" s="20"/>
     </row>
     <row r="158" spans="1:13" x14ac:dyDescent="0.25">
@@ -6606,7 +7358,9 @@
       </c>
       <c r="J158" s="20"/>
       <c r="K158" s="20"/>
-      <c r="L158" s="20"/>
+      <c r="L158" s="20" t="s">
+        <v>18</v>
+      </c>
       <c r="M158" s="20"/>
     </row>
     <row r="159" spans="1:13" x14ac:dyDescent="0.25">
@@ -6641,7 +7395,9 @@
       </c>
       <c r="J159" s="20"/>
       <c r="K159" s="20"/>
-      <c r="L159" s="20"/>
+      <c r="L159" s="20" t="s">
+        <v>18</v>
+      </c>
       <c r="M159" s="20"/>
     </row>
     <row r="160" spans="1:13" x14ac:dyDescent="0.25">
@@ -6676,7 +7432,9 @@
       </c>
       <c r="J160" s="20"/>
       <c r="K160" s="20"/>
-      <c r="L160" s="20"/>
+      <c r="L160" s="20" t="s">
+        <v>18</v>
+      </c>
       <c r="M160" s="20"/>
     </row>
     <row r="161" spans="1:13" x14ac:dyDescent="0.25">
@@ -6711,7 +7469,9 @@
       </c>
       <c r="J161" s="20"/>
       <c r="K161" s="20"/>
-      <c r="L161" s="20"/>
+      <c r="L161" s="20" t="s">
+        <v>18</v>
+      </c>
       <c r="M161" s="20"/>
     </row>
     <row r="162" spans="1:13" x14ac:dyDescent="0.25">
@@ -6746,7 +7506,9 @@
       </c>
       <c r="J162" s="20"/>
       <c r="K162" s="20"/>
-      <c r="L162" s="20"/>
+      <c r="L162" s="20" t="s">
+        <v>18</v>
+      </c>
       <c r="M162" s="20"/>
     </row>
     <row r="163" spans="1:13" x14ac:dyDescent="0.25">
@@ -6781,7 +7543,9 @@
       </c>
       <c r="J163" s="20"/>
       <c r="K163" s="20"/>
-      <c r="L163" s="20"/>
+      <c r="L163" s="20" t="s">
+        <v>18</v>
+      </c>
       <c r="M163" s="20"/>
     </row>
     <row r="164" spans="1:13" x14ac:dyDescent="0.25">
@@ -6816,7 +7580,9 @@
       </c>
       <c r="J164" s="20"/>
       <c r="K164" s="20"/>
-      <c r="L164" s="20"/>
+      <c r="L164" s="20" t="s">
+        <v>18</v>
+      </c>
       <c r="M164" s="20"/>
     </row>
     <row r="165" spans="1:13" x14ac:dyDescent="0.25">
@@ -6851,7 +7617,9 @@
       </c>
       <c r="J165" s="20"/>
       <c r="K165" s="20"/>
-      <c r="L165" s="20"/>
+      <c r="L165" s="20" t="s">
+        <v>18</v>
+      </c>
       <c r="M165" s="20"/>
     </row>
     <row r="166" spans="1:13" x14ac:dyDescent="0.25">
@@ -6886,7 +7654,9 @@
       </c>
       <c r="J166" s="20"/>
       <c r="K166" s="20"/>
-      <c r="L166" s="20"/>
+      <c r="L166" s="20" t="s">
+        <v>18</v>
+      </c>
       <c r="M166" s="20"/>
     </row>
     <row r="167" spans="1:13" x14ac:dyDescent="0.25">
@@ -6921,7 +7691,9 @@
       </c>
       <c r="J167" s="20"/>
       <c r="K167" s="20"/>
-      <c r="L167" s="20"/>
+      <c r="L167" s="20" t="s">
+        <v>18</v>
+      </c>
       <c r="M167" s="20"/>
     </row>
     <row r="168" spans="1:13" x14ac:dyDescent="0.25">
@@ -6956,7 +7728,9 @@
       </c>
       <c r="J168" s="20"/>
       <c r="K168" s="20"/>
-      <c r="L168" s="20"/>
+      <c r="L168" s="20" t="s">
+        <v>18</v>
+      </c>
       <c r="M168" s="20"/>
     </row>
     <row r="169" spans="1:13" x14ac:dyDescent="0.25">
@@ -6991,7 +7765,9 @@
       </c>
       <c r="J169" s="20"/>
       <c r="K169" s="20"/>
-      <c r="L169" s="20"/>
+      <c r="L169" s="20" t="s">
+        <v>18</v>
+      </c>
       <c r="M169" s="20"/>
     </row>
     <row r="170" spans="1:13" x14ac:dyDescent="0.25">
@@ -7026,7 +7802,9 @@
       </c>
       <c r="J170" s="20"/>
       <c r="K170" s="20"/>
-      <c r="L170" s="20"/>
+      <c r="L170" s="20" t="s">
+        <v>18</v>
+      </c>
       <c r="M170" s="20"/>
     </row>
     <row r="171" spans="1:13" x14ac:dyDescent="0.25">
@@ -7056,7 +7834,9 @@
       </c>
       <c r="J171" s="18"/>
       <c r="K171" s="18"/>
-      <c r="L171" s="18"/>
+      <c r="L171" s="18" t="s">
+        <v>18</v>
+      </c>
       <c r="M171" s="18"/>
     </row>
     <row r="172" spans="1:13" x14ac:dyDescent="0.25">
@@ -7086,7 +7866,9 @@
       </c>
       <c r="J172" s="18"/>
       <c r="K172" s="18"/>
-      <c r="L172" s="18"/>
+      <c r="L172" s="18" t="s">
+        <v>18</v>
+      </c>
       <c r="M172" s="18"/>
     </row>
     <row r="173" spans="1:13" x14ac:dyDescent="0.25">
@@ -7116,7 +7898,9 @@
       </c>
       <c r="J173" s="18"/>
       <c r="K173" s="18"/>
-      <c r="L173" s="18"/>
+      <c r="L173" s="18" t="s">
+        <v>18</v>
+      </c>
       <c r="M173" s="18"/>
     </row>
     <row r="174" spans="1:13" x14ac:dyDescent="0.25">
@@ -7146,8 +7930,2750 @@
       </c>
       <c r="J174" s="18"/>
       <c r="K174" s="18"/>
-      <c r="L174" s="18"/>
+      <c r="L174" s="18" t="s">
+        <v>18</v>
+      </c>
       <c r="M174" s="18"/>
+    </row>
+    <row r="175" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A175" s="42" t="s">
+        <v>87</v>
+      </c>
+      <c r="B175" s="42" t="s">
+        <v>40</v>
+      </c>
+      <c r="C175" s="42" t="s">
+        <v>86</v>
+      </c>
+      <c r="D175" s="42" t="s">
+        <v>1</v>
+      </c>
+      <c r="E175" s="42">
+        <v>2012</v>
+      </c>
+      <c r="F175" s="42"/>
+      <c r="G175" s="42"/>
+      <c r="H175" s="42">
+        <v>0.9</v>
+      </c>
+      <c r="I175" s="42"/>
+      <c r="J175" s="42"/>
+      <c r="K175" s="42"/>
+      <c r="L175" s="42" t="s">
+        <v>83</v>
+      </c>
+      <c r="M175" s="42"/>
+    </row>
+    <row r="176" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A176" s="42" t="s">
+        <v>87</v>
+      </c>
+      <c r="B176" s="42" t="s">
+        <v>40</v>
+      </c>
+      <c r="C176" s="42" t="s">
+        <v>86</v>
+      </c>
+      <c r="D176" s="42" t="s">
+        <v>2</v>
+      </c>
+      <c r="E176" s="42">
+        <v>2012</v>
+      </c>
+      <c r="F176" s="42"/>
+      <c r="G176" s="42"/>
+      <c r="H176" s="42">
+        <v>1.3</v>
+      </c>
+      <c r="I176" s="42"/>
+      <c r="J176" s="42"/>
+      <c r="K176" s="42"/>
+      <c r="L176" s="42" t="s">
+        <v>83</v>
+      </c>
+      <c r="M176" s="42"/>
+    </row>
+    <row r="177" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A177" s="42" t="s">
+        <v>87</v>
+      </c>
+      <c r="B177" s="42" t="s">
+        <v>40</v>
+      </c>
+      <c r="C177" s="42" t="s">
+        <v>86</v>
+      </c>
+      <c r="D177" s="42" t="s">
+        <v>3</v>
+      </c>
+      <c r="E177" s="42">
+        <v>2012</v>
+      </c>
+      <c r="F177" s="42"/>
+      <c r="G177" s="42"/>
+      <c r="H177" s="42">
+        <v>4.3</v>
+      </c>
+      <c r="I177" s="42"/>
+      <c r="J177" s="42"/>
+      <c r="K177" s="42"/>
+      <c r="L177" s="42" t="s">
+        <v>83</v>
+      </c>
+      <c r="M177" s="42"/>
+    </row>
+    <row r="178" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A178" s="42" t="s">
+        <v>87</v>
+      </c>
+      <c r="B178" s="42" t="s">
+        <v>40</v>
+      </c>
+      <c r="C178" s="42" t="s">
+        <v>86</v>
+      </c>
+      <c r="D178" s="42" t="s">
+        <v>4</v>
+      </c>
+      <c r="E178" s="42">
+        <v>2012</v>
+      </c>
+      <c r="F178" s="42"/>
+      <c r="G178" s="42"/>
+      <c r="H178" s="42">
+        <v>6.6</v>
+      </c>
+      <c r="I178" s="42"/>
+      <c r="J178" s="42"/>
+      <c r="K178" s="42"/>
+      <c r="L178" s="42" t="s">
+        <v>83</v>
+      </c>
+      <c r="M178" s="42"/>
+    </row>
+    <row r="179" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A179" s="42" t="s">
+        <v>87</v>
+      </c>
+      <c r="B179" s="42" t="s">
+        <v>40</v>
+      </c>
+      <c r="C179" s="42" t="s">
+        <v>86</v>
+      </c>
+      <c r="D179" s="42" t="s">
+        <v>5</v>
+      </c>
+      <c r="E179" s="42">
+        <v>2012</v>
+      </c>
+      <c r="F179" s="42"/>
+      <c r="G179" s="42"/>
+      <c r="H179" s="42">
+        <v>5</v>
+      </c>
+      <c r="I179" s="42"/>
+      <c r="J179" s="42"/>
+      <c r="K179" s="42"/>
+      <c r="L179" s="42" t="s">
+        <v>83</v>
+      </c>
+      <c r="M179" s="42"/>
+    </row>
+    <row r="180" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A180" s="42" t="s">
+        <v>87</v>
+      </c>
+      <c r="B180" s="42" t="s">
+        <v>40</v>
+      </c>
+      <c r="C180" s="42" t="s">
+        <v>86</v>
+      </c>
+      <c r="D180" s="42" t="s">
+        <v>6</v>
+      </c>
+      <c r="E180" s="42">
+        <v>2012</v>
+      </c>
+      <c r="F180" s="42"/>
+      <c r="G180" s="42"/>
+      <c r="H180" s="42">
+        <v>8.1</v>
+      </c>
+      <c r="I180" s="42"/>
+      <c r="J180" s="42"/>
+      <c r="K180" s="42"/>
+      <c r="L180" s="42" t="s">
+        <v>83</v>
+      </c>
+      <c r="M180" s="42"/>
+    </row>
+    <row r="181" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A181" s="42" t="s">
+        <v>87</v>
+      </c>
+      <c r="B181" s="42" t="s">
+        <v>40</v>
+      </c>
+      <c r="C181" s="42" t="s">
+        <v>86</v>
+      </c>
+      <c r="D181" s="42" t="s">
+        <v>7</v>
+      </c>
+      <c r="E181" s="42">
+        <v>2012</v>
+      </c>
+      <c r="F181" s="42"/>
+      <c r="G181" s="42"/>
+      <c r="H181" s="42">
+        <v>8.9</v>
+      </c>
+      <c r="I181" s="42"/>
+      <c r="J181" s="42"/>
+      <c r="K181" s="42"/>
+      <c r="L181" s="42" t="s">
+        <v>83</v>
+      </c>
+      <c r="M181" s="42"/>
+    </row>
+    <row r="182" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A182" s="42" t="s">
+        <v>87</v>
+      </c>
+      <c r="B182" s="42" t="s">
+        <v>40</v>
+      </c>
+      <c r="C182" s="42" t="s">
+        <v>86</v>
+      </c>
+      <c r="D182" s="42" t="s">
+        <v>32</v>
+      </c>
+      <c r="E182" s="42">
+        <v>2012</v>
+      </c>
+      <c r="F182" s="42"/>
+      <c r="G182" s="42"/>
+      <c r="H182" s="42">
+        <v>7</v>
+      </c>
+      <c r="I182" s="42"/>
+      <c r="J182" s="42"/>
+      <c r="K182" s="42"/>
+      <c r="L182" s="42" t="s">
+        <v>83</v>
+      </c>
+      <c r="M182" s="42"/>
+    </row>
+    <row r="183" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A183" s="42" t="s">
+        <v>87</v>
+      </c>
+      <c r="B183" s="42" t="s">
+        <v>40</v>
+      </c>
+      <c r="C183" s="42" t="s">
+        <v>86</v>
+      </c>
+      <c r="D183" s="42" t="s">
+        <v>36</v>
+      </c>
+      <c r="E183" s="42">
+        <v>2012</v>
+      </c>
+      <c r="F183" s="42"/>
+      <c r="G183" s="42"/>
+      <c r="H183" s="42">
+        <v>4</v>
+      </c>
+      <c r="I183" s="42"/>
+      <c r="J183" s="42"/>
+      <c r="K183" s="42"/>
+      <c r="L183" s="42" t="s">
+        <v>83</v>
+      </c>
+      <c r="M183" s="42"/>
+    </row>
+    <row r="184" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A184" s="42" t="s">
+        <v>87</v>
+      </c>
+      <c r="B184" s="42" t="s">
+        <v>40</v>
+      </c>
+      <c r="C184" s="42" t="s">
+        <v>86</v>
+      </c>
+      <c r="D184" s="42" t="s">
+        <v>37</v>
+      </c>
+      <c r="E184" s="42">
+        <v>2012</v>
+      </c>
+      <c r="F184" s="42"/>
+      <c r="G184" s="42"/>
+      <c r="H184" s="42">
+        <v>5</v>
+      </c>
+      <c r="I184" s="42"/>
+      <c r="J184" s="42"/>
+      <c r="K184" s="42"/>
+      <c r="L184" s="42" t="s">
+        <v>83</v>
+      </c>
+      <c r="M184" s="42"/>
+    </row>
+    <row r="185" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A185" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B185" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C185" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="D185" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E185" s="3">
+        <v>2012</v>
+      </c>
+      <c r="F185" s="3"/>
+      <c r="G185" s="3"/>
+      <c r="H185" s="3">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="I185" s="3"/>
+      <c r="J185" s="3"/>
+      <c r="K185" s="3"/>
+      <c r="L185" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="M185" s="3"/>
+    </row>
+    <row r="186" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A186" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B186" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C186" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="D186" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E186" s="3">
+        <v>2012</v>
+      </c>
+      <c r="F186" s="3"/>
+      <c r="G186" s="3"/>
+      <c r="H186" s="3">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="I186" s="3"/>
+      <c r="J186" s="3"/>
+      <c r="K186" s="3"/>
+      <c r="L186" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="M186" s="3"/>
+    </row>
+    <row r="187" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A187" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B187" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C187" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="D187" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E187" s="3">
+        <v>2012</v>
+      </c>
+      <c r="F187" s="3"/>
+      <c r="G187" s="3"/>
+      <c r="H187" s="3">
+        <v>7.9</v>
+      </c>
+      <c r="I187" s="3"/>
+      <c r="J187" s="3"/>
+      <c r="K187" s="3"/>
+      <c r="L187" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="M187" s="3"/>
+    </row>
+    <row r="188" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A188" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B188" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C188" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="D188" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E188" s="3">
+        <v>2012</v>
+      </c>
+      <c r="F188" s="3"/>
+      <c r="G188" s="3"/>
+      <c r="H188" s="3">
+        <v>6.6</v>
+      </c>
+      <c r="I188" s="3"/>
+      <c r="J188" s="3"/>
+      <c r="K188" s="3"/>
+      <c r="L188" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="M188" s="3"/>
+    </row>
+    <row r="189" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A189" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B189" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C189" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="D189" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E189" s="3">
+        <v>2012</v>
+      </c>
+      <c r="F189" s="3"/>
+      <c r="G189" s="3"/>
+      <c r="H189" s="3">
+        <v>12.3</v>
+      </c>
+      <c r="I189" s="3"/>
+      <c r="J189" s="3"/>
+      <c r="K189" s="3"/>
+      <c r="L189" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="M189" s="3"/>
+    </row>
+    <row r="190" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A190" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B190" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C190" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="D190" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E190" s="3">
+        <v>2012</v>
+      </c>
+      <c r="F190" s="3"/>
+      <c r="G190" s="3"/>
+      <c r="H190" s="3">
+        <v>10.6</v>
+      </c>
+      <c r="I190" s="3"/>
+      <c r="J190" s="3"/>
+      <c r="K190" s="3"/>
+      <c r="L190" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="M190" s="3"/>
+    </row>
+    <row r="191" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A191" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B191" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C191" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="D191" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E191" s="3">
+        <v>2012</v>
+      </c>
+      <c r="F191" s="3"/>
+      <c r="G191" s="3"/>
+      <c r="H191" s="3">
+        <v>10.7</v>
+      </c>
+      <c r="I191" s="3"/>
+      <c r="J191" s="3"/>
+      <c r="K191" s="3"/>
+      <c r="L191" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="M191" s="3"/>
+    </row>
+    <row r="192" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A192" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B192" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C192" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="D192" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E192" s="3">
+        <v>2012</v>
+      </c>
+      <c r="F192" s="3"/>
+      <c r="G192" s="3"/>
+      <c r="H192" s="3">
+        <v>10</v>
+      </c>
+      <c r="I192" s="3"/>
+      <c r="J192" s="3"/>
+      <c r="K192" s="3"/>
+      <c r="L192" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="M192" s="3"/>
+    </row>
+    <row r="193" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A193" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B193" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C193" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="D193" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E193" s="3">
+        <v>2012</v>
+      </c>
+      <c r="F193" s="3"/>
+      <c r="G193" s="3"/>
+      <c r="H193" s="3">
+        <v>5</v>
+      </c>
+      <c r="I193" s="3"/>
+      <c r="J193" s="3"/>
+      <c r="K193" s="3"/>
+      <c r="L193" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="M193" s="3"/>
+    </row>
+    <row r="194" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A194" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B194" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C194" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="D194" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E194" s="3">
+        <v>2012</v>
+      </c>
+      <c r="F194" s="3"/>
+      <c r="G194" s="3"/>
+      <c r="H194" s="3">
+        <v>3</v>
+      </c>
+      <c r="I194" s="3"/>
+      <c r="J194" s="3"/>
+      <c r="K194" s="3"/>
+      <c r="L194" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="M194" s="3"/>
+    </row>
+    <row r="195" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A195" s="26" t="s">
+        <v>85</v>
+      </c>
+      <c r="B195" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="C195" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="D195" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="E195" s="26">
+        <v>1990</v>
+      </c>
+      <c r="F195" s="26"/>
+      <c r="G195" s="26"/>
+      <c r="H195" s="26">
+        <v>3.8</v>
+      </c>
+      <c r="I195" s="44">
+        <f>(Table1[[#This Row],[UB]]-Table1[[#This Row],[LB]])/3.92</f>
+        <v>0.3061224489795919</v>
+      </c>
+      <c r="J195" s="40">
+        <v>3.2</v>
+      </c>
+      <c r="K195" s="26">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="L195" s="26" t="s">
+        <v>83</v>
+      </c>
+      <c r="M195" s="26"/>
+    </row>
+    <row r="196" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A196" s="26" t="s">
+        <v>85</v>
+      </c>
+      <c r="B196" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="C196" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="D196" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="E196" s="26">
+        <v>1991</v>
+      </c>
+      <c r="F196" s="26"/>
+      <c r="G196" s="26"/>
+      <c r="H196" s="26">
+        <v>4.8</v>
+      </c>
+      <c r="I196" s="44">
+        <f>(Table1[[#This Row],[UB]]-Table1[[#This Row],[LB]])/3.92</f>
+        <v>0.40816326530612235</v>
+      </c>
+      <c r="J196" s="40">
+        <v>4</v>
+      </c>
+      <c r="K196" s="26">
+        <v>5.6</v>
+      </c>
+      <c r="L196" s="26" t="s">
+        <v>83</v>
+      </c>
+      <c r="M196" s="26"/>
+    </row>
+    <row r="197" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A197" s="26" t="s">
+        <v>85</v>
+      </c>
+      <c r="B197" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="C197" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="D197" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="E197" s="26">
+        <v>1992</v>
+      </c>
+      <c r="F197" s="26"/>
+      <c r="G197" s="26"/>
+      <c r="H197" s="26">
+        <v>5.8</v>
+      </c>
+      <c r="I197" s="44">
+        <f>(Table1[[#This Row],[UB]]-Table1[[#This Row],[LB]])/3.92</f>
+        <v>0.4846938775510205</v>
+      </c>
+      <c r="J197" s="40">
+        <v>4.8</v>
+      </c>
+      <c r="K197" s="26">
+        <v>6.7</v>
+      </c>
+      <c r="L197" s="26" t="s">
+        <v>83</v>
+      </c>
+      <c r="M197" s="26"/>
+    </row>
+    <row r="198" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A198" s="26" t="s">
+        <v>85</v>
+      </c>
+      <c r="B198" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="C198" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="D198" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="E198" s="26">
+        <v>1993</v>
+      </c>
+      <c r="F198" s="26"/>
+      <c r="G198" s="26"/>
+      <c r="H198" s="26">
+        <v>6.6</v>
+      </c>
+      <c r="I198" s="44">
+        <f>(Table1[[#This Row],[UB]]-Table1[[#This Row],[LB]])/3.92</f>
+        <v>0.53571428571428559</v>
+      </c>
+      <c r="J198" s="40">
+        <v>5.5</v>
+      </c>
+      <c r="K198" s="26">
+        <v>7.6</v>
+      </c>
+      <c r="L198" s="26" t="s">
+        <v>83</v>
+      </c>
+      <c r="M198" s="26"/>
+    </row>
+    <row r="199" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A199" s="26" t="s">
+        <v>85</v>
+      </c>
+      <c r="B199" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="C199" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="D199" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="E199" s="26">
+        <v>1994</v>
+      </c>
+      <c r="F199" s="26"/>
+      <c r="G199" s="26"/>
+      <c r="H199" s="26">
+        <v>7.2</v>
+      </c>
+      <c r="I199" s="44">
+        <f>(Table1[[#This Row],[UB]]-Table1[[#This Row],[LB]])/3.92</f>
+        <v>0.58673469387755117</v>
+      </c>
+      <c r="J199" s="40">
+        <v>6</v>
+      </c>
+      <c r="K199" s="26">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="L199" s="26" t="s">
+        <v>83</v>
+      </c>
+      <c r="M199" s="26"/>
+    </row>
+    <row r="200" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A200" s="26" t="s">
+        <v>85</v>
+      </c>
+      <c r="B200" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="C200" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="D200" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="E200" s="26">
+        <v>1995</v>
+      </c>
+      <c r="F200" s="26"/>
+      <c r="G200" s="26"/>
+      <c r="H200" s="26">
+        <v>7.6</v>
+      </c>
+      <c r="I200" s="44">
+        <f>(Table1[[#This Row],[UB]]-Table1[[#This Row],[LB]])/3.92</f>
+        <v>0.63775510204081609</v>
+      </c>
+      <c r="J200" s="40">
+        <v>6.2</v>
+      </c>
+      <c r="K200" s="26">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="L200" s="26" t="s">
+        <v>83</v>
+      </c>
+      <c r="M200" s="26"/>
+    </row>
+    <row r="201" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A201" s="26" t="s">
+        <v>85</v>
+      </c>
+      <c r="B201" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="C201" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="D201" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="E201" s="26">
+        <v>1996</v>
+      </c>
+      <c r="F201" s="26"/>
+      <c r="G201" s="26"/>
+      <c r="H201" s="26">
+        <v>7.7</v>
+      </c>
+      <c r="I201" s="44">
+        <f>(Table1[[#This Row],[UB]]-Table1[[#This Row],[LB]])/3.92</f>
+        <v>0.63775510204081653</v>
+      </c>
+      <c r="J201" s="40">
+        <v>6.3</v>
+      </c>
+      <c r="K201" s="26">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="L201" s="26" t="s">
+        <v>83</v>
+      </c>
+      <c r="M201" s="26"/>
+    </row>
+    <row r="202" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A202" s="26" t="s">
+        <v>85</v>
+      </c>
+      <c r="B202" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="C202" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="D202" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="E202" s="26">
+        <v>1997</v>
+      </c>
+      <c r="F202" s="26"/>
+      <c r="G202" s="26"/>
+      <c r="H202" s="26">
+        <v>7.6</v>
+      </c>
+      <c r="I202" s="44">
+        <f>(Table1[[#This Row],[UB]]-Table1[[#This Row],[LB]])/3.92</f>
+        <v>0.63775510204081653</v>
+      </c>
+      <c r="J202" s="40">
+        <v>6.3</v>
+      </c>
+      <c r="K202" s="26">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="L202" s="26" t="s">
+        <v>83</v>
+      </c>
+      <c r="M202" s="26"/>
+    </row>
+    <row r="203" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A203" s="26" t="s">
+        <v>85</v>
+      </c>
+      <c r="B203" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="C203" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="D203" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="E203" s="26">
+        <v>1998</v>
+      </c>
+      <c r="F203" s="26"/>
+      <c r="G203" s="26"/>
+      <c r="H203" s="26">
+        <v>7.4</v>
+      </c>
+      <c r="I203" s="44">
+        <f>(Table1[[#This Row],[UB]]-Table1[[#This Row],[LB]])/3.92</f>
+        <v>0.6122448979591838</v>
+      </c>
+      <c r="J203" s="40">
+        <v>6.1</v>
+      </c>
+      <c r="K203" s="26">
+        <v>8.5</v>
+      </c>
+      <c r="L203" s="26" t="s">
+        <v>83</v>
+      </c>
+      <c r="M203" s="26"/>
+    </row>
+    <row r="204" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A204" s="26" t="s">
+        <v>85</v>
+      </c>
+      <c r="B204" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="C204" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="D204" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="E204" s="26">
+        <v>1999</v>
+      </c>
+      <c r="F204" s="26"/>
+      <c r="G204" s="26"/>
+      <c r="H204" s="26">
+        <v>7.1</v>
+      </c>
+      <c r="I204" s="44">
+        <f>(Table1[[#This Row],[UB]]-Table1[[#This Row],[LB]])/3.92</f>
+        <v>0.61224489795918358</v>
+      </c>
+      <c r="J204" s="40">
+        <v>5.8</v>
+      </c>
+      <c r="K204" s="26">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="L204" s="26" t="s">
+        <v>83</v>
+      </c>
+      <c r="M204" s="26"/>
+    </row>
+    <row r="205" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A205" s="26" t="s">
+        <v>85</v>
+      </c>
+      <c r="B205" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="C205" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="D205" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="E205" s="26">
+        <v>2000</v>
+      </c>
+      <c r="F205" s="26"/>
+      <c r="G205" s="26"/>
+      <c r="H205" s="26">
+        <v>6.7</v>
+      </c>
+      <c r="I205" s="44">
+        <f>(Table1[[#This Row],[UB]]-Table1[[#This Row],[LB]])/3.92</f>
+        <v>0.58673469387755095</v>
+      </c>
+      <c r="J205" s="40">
+        <v>5.5</v>
+      </c>
+      <c r="K205" s="26">
+        <v>7.8</v>
+      </c>
+      <c r="L205" s="26" t="s">
+        <v>83</v>
+      </c>
+      <c r="M205" s="26"/>
+    </row>
+    <row r="206" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A206" s="26" t="s">
+        <v>85</v>
+      </c>
+      <c r="B206" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="C206" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="D206" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="E206" s="26">
+        <v>2001</v>
+      </c>
+      <c r="F206" s="26"/>
+      <c r="G206" s="26"/>
+      <c r="H206" s="26">
+        <v>6.3</v>
+      </c>
+      <c r="I206" s="44">
+        <f>(Table1[[#This Row],[UB]]-Table1[[#This Row],[LB]])/3.92</f>
+        <v>0.53571428571428559</v>
+      </c>
+      <c r="J206" s="40">
+        <v>5.2</v>
+      </c>
+      <c r="K206" s="26">
+        <v>7.3</v>
+      </c>
+      <c r="L206" s="26" t="s">
+        <v>83</v>
+      </c>
+      <c r="M206" s="26"/>
+    </row>
+    <row r="207" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A207" s="26" t="s">
+        <v>85</v>
+      </c>
+      <c r="B207" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="C207" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="D207" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="E207" s="26">
+        <v>2002</v>
+      </c>
+      <c r="F207" s="26"/>
+      <c r="G207" s="26"/>
+      <c r="H207" s="26">
+        <v>5.9</v>
+      </c>
+      <c r="I207" s="44">
+        <f>(Table1[[#This Row],[UB]]-Table1[[#This Row],[LB]])/3.92</f>
+        <v>0.48469387755102028</v>
+      </c>
+      <c r="J207" s="40">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="K207" s="26">
+        <v>6.8</v>
+      </c>
+      <c r="L207" s="26" t="s">
+        <v>83</v>
+      </c>
+      <c r="M207" s="26"/>
+    </row>
+    <row r="208" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A208" s="26" t="s">
+        <v>85</v>
+      </c>
+      <c r="B208" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="C208" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="D208" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="E208" s="26">
+        <v>2003</v>
+      </c>
+      <c r="F208" s="26"/>
+      <c r="G208" s="26"/>
+      <c r="H208" s="26">
+        <v>5.5</v>
+      </c>
+      <c r="I208" s="44">
+        <f>(Table1[[#This Row],[UB]]-Table1[[#This Row],[LB]])/3.92</f>
+        <v>0.45918367346938793</v>
+      </c>
+      <c r="J208" s="40">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="K208" s="26">
+        <v>6.4</v>
+      </c>
+      <c r="L208" s="26" t="s">
+        <v>83</v>
+      </c>
+      <c r="M208" s="26"/>
+    </row>
+    <row r="209" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A209" s="26" t="s">
+        <v>85</v>
+      </c>
+      <c r="B209" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="C209" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="D209" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="E209" s="26">
+        <v>2004</v>
+      </c>
+      <c r="F209" s="26"/>
+      <c r="G209" s="26"/>
+      <c r="H209" s="26">
+        <v>5.2</v>
+      </c>
+      <c r="I209" s="44">
+        <f>(Table1[[#This Row],[UB]]-Table1[[#This Row],[LB]])/3.92</f>
+        <v>0.43367346938775514</v>
+      </c>
+      <c r="J209" s="40">
+        <v>4.3</v>
+      </c>
+      <c r="K209" s="26">
+        <v>6</v>
+      </c>
+      <c r="L209" s="26" t="s">
+        <v>83</v>
+      </c>
+      <c r="M209" s="26"/>
+    </row>
+    <row r="210" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A210" s="26" t="s">
+        <v>85</v>
+      </c>
+      <c r="B210" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="C210" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="D210" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="E210" s="26">
+        <v>2005</v>
+      </c>
+      <c r="F210" s="26"/>
+      <c r="G210" s="26"/>
+      <c r="H210" s="26">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="I210" s="44">
+        <f>(Table1[[#This Row],[UB]]-Table1[[#This Row],[LB]])/3.92</f>
+        <v>0.43367346938775514</v>
+      </c>
+      <c r="J210" s="40">
+        <v>4</v>
+      </c>
+      <c r="K210" s="26">
+        <v>5.7</v>
+      </c>
+      <c r="L210" s="26" t="s">
+        <v>83</v>
+      </c>
+      <c r="M210" s="26"/>
+    </row>
+    <row r="211" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A211" s="26" t="s">
+        <v>85</v>
+      </c>
+      <c r="B211" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="C211" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="D211" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="E211" s="26">
+        <v>2006</v>
+      </c>
+      <c r="F211" s="26"/>
+      <c r="G211" s="26"/>
+      <c r="H211" s="26">
+        <v>4.7</v>
+      </c>
+      <c r="I211" s="44">
+        <f>(Table1[[#This Row],[UB]]-Table1[[#This Row],[LB]])/3.92</f>
+        <v>0.38265306122448994</v>
+      </c>
+      <c r="J211" s="40">
+        <v>3.9</v>
+      </c>
+      <c r="K211" s="26">
+        <v>5.4</v>
+      </c>
+      <c r="L211" s="26" t="s">
+        <v>83</v>
+      </c>
+      <c r="M211" s="26"/>
+    </row>
+    <row r="212" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A212" s="26" t="s">
+        <v>85</v>
+      </c>
+      <c r="B212" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="C212" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="D212" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="E212" s="26">
+        <v>2007</v>
+      </c>
+      <c r="F212" s="26"/>
+      <c r="G212" s="26"/>
+      <c r="H212" s="26">
+        <v>4.5</v>
+      </c>
+      <c r="I212" s="44">
+        <f>(Table1[[#This Row],[UB]]-Table1[[#This Row],[LB]])/3.92</f>
+        <v>0.38265306122448978</v>
+      </c>
+      <c r="J212" s="40">
+        <v>3.7</v>
+      </c>
+      <c r="K212" s="26">
+        <v>5.2</v>
+      </c>
+      <c r="L212" s="26" t="s">
+        <v>83</v>
+      </c>
+      <c r="M212" s="26"/>
+    </row>
+    <row r="213" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A213" s="26" t="s">
+        <v>85</v>
+      </c>
+      <c r="B213" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="C213" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="D213" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="E213" s="26">
+        <v>2008</v>
+      </c>
+      <c r="F213" s="26"/>
+      <c r="G213" s="26"/>
+      <c r="H213" s="26">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="I213" s="44">
+        <f>(Table1[[#This Row],[UB]]-Table1[[#This Row],[LB]])/3.92</f>
+        <v>0.38265306122448967</v>
+      </c>
+      <c r="J213" s="40">
+        <v>3.6</v>
+      </c>
+      <c r="K213" s="26">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="L213" s="26" t="s">
+        <v>83</v>
+      </c>
+      <c r="M213" s="26"/>
+    </row>
+    <row r="214" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A214" s="26" t="s">
+        <v>85</v>
+      </c>
+      <c r="B214" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="C214" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="D214" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="E214" s="26">
+        <v>2009</v>
+      </c>
+      <c r="F214" s="26"/>
+      <c r="G214" s="26"/>
+      <c r="H214" s="26">
+        <v>4.3</v>
+      </c>
+      <c r="I214" s="44">
+        <f>(Table1[[#This Row],[UB]]-Table1[[#This Row],[LB]])/3.92</f>
+        <v>0.35714285714285715</v>
+      </c>
+      <c r="J214" s="40">
+        <v>3.6</v>
+      </c>
+      <c r="K214" s="26">
+        <v>5</v>
+      </c>
+      <c r="L214" s="26" t="s">
+        <v>83</v>
+      </c>
+      <c r="M214" s="26"/>
+    </row>
+    <row r="215" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A215" s="26" t="s">
+        <v>85</v>
+      </c>
+      <c r="B215" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="C215" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="D215" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="E215" s="26">
+        <v>2010</v>
+      </c>
+      <c r="F215" s="26"/>
+      <c r="G215" s="26"/>
+      <c r="H215" s="26">
+        <v>4.2</v>
+      </c>
+      <c r="I215" s="44">
+        <f>(Table1[[#This Row],[UB]]-Table1[[#This Row],[LB]])/3.92</f>
+        <v>0.35714285714285726</v>
+      </c>
+      <c r="J215" s="40">
+        <v>3.5</v>
+      </c>
+      <c r="K215" s="26">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="L215" s="26" t="s">
+        <v>83</v>
+      </c>
+      <c r="M215" s="26"/>
+    </row>
+    <row r="216" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A216" s="26" t="s">
+        <v>85</v>
+      </c>
+      <c r="B216" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="C216" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="D216" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="E216" s="26">
+        <v>2011</v>
+      </c>
+      <c r="F216" s="26"/>
+      <c r="G216" s="26"/>
+      <c r="H216" s="26">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="I216" s="44">
+        <f>(Table1[[#This Row],[UB]]-Table1[[#This Row],[LB]])/3.92</f>
+        <v>0.35714285714285715</v>
+      </c>
+      <c r="J216" s="40">
+        <v>3.4</v>
+      </c>
+      <c r="K216" s="26">
+        <v>4.8</v>
+      </c>
+      <c r="L216" s="26" t="s">
+        <v>83</v>
+      </c>
+      <c r="M216" s="26"/>
+    </row>
+    <row r="217" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A217" s="26" t="s">
+        <v>85</v>
+      </c>
+      <c r="B217" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="C217" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="D217" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="E217" s="26">
+        <v>2012</v>
+      </c>
+      <c r="F217" s="26"/>
+      <c r="G217" s="26"/>
+      <c r="H217" s="26">
+        <v>4</v>
+      </c>
+      <c r="I217" s="44">
+        <f>(Table1[[#This Row],[UB]]-Table1[[#This Row],[LB]])/3.92</f>
+        <v>0.35714285714285726</v>
+      </c>
+      <c r="J217" s="40">
+        <v>3.3</v>
+      </c>
+      <c r="K217" s="26">
+        <v>4.7</v>
+      </c>
+      <c r="L217" s="26" t="s">
+        <v>83</v>
+      </c>
+      <c r="M217" s="26"/>
+    </row>
+    <row r="218" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A218" s="26" t="s">
+        <v>85</v>
+      </c>
+      <c r="B218" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="C218" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="D218" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="E218" s="26">
+        <v>2013</v>
+      </c>
+      <c r="F218" s="26"/>
+      <c r="G218" s="26"/>
+      <c r="H218" s="26">
+        <v>3.9</v>
+      </c>
+      <c r="I218" s="44">
+        <f>(Table1[[#This Row],[UB]]-Table1[[#This Row],[LB]])/3.92</f>
+        <v>0.33163265306122447</v>
+      </c>
+      <c r="J218" s="40">
+        <v>3.2</v>
+      </c>
+      <c r="K218" s="26">
+        <v>4.5</v>
+      </c>
+      <c r="L218" s="26" t="s">
+        <v>83</v>
+      </c>
+      <c r="M218" s="26"/>
+    </row>
+    <row r="219" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A219" s="26" t="s">
+        <v>85</v>
+      </c>
+      <c r="B219" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="C219" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="D219" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="E219" s="26">
+        <v>2014</v>
+      </c>
+      <c r="F219" s="26"/>
+      <c r="G219" s="26"/>
+      <c r="H219" s="26">
+        <v>3.8</v>
+      </c>
+      <c r="I219" s="44">
+        <f>(Table1[[#This Row],[UB]]-Table1[[#This Row],[LB]])/3.92</f>
+        <v>0.33163265306122458</v>
+      </c>
+      <c r="J219" s="40">
+        <v>3.1</v>
+      </c>
+      <c r="K219" s="26">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="L219" s="26" t="s">
+        <v>83</v>
+      </c>
+      <c r="M219" s="26"/>
+    </row>
+    <row r="220" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A220" s="26" t="s">
+        <v>85</v>
+      </c>
+      <c r="B220" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="C220" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="D220" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="E220" s="26">
+        <v>2015</v>
+      </c>
+      <c r="F220" s="26"/>
+      <c r="G220" s="26"/>
+      <c r="H220" s="26">
+        <v>3.7</v>
+      </c>
+      <c r="I220" s="44">
+        <f>(Table1[[#This Row],[UB]]-Table1[[#This Row],[LB]])/3.92</f>
+        <v>0.33163265306122447</v>
+      </c>
+      <c r="J220" s="40">
+        <v>3</v>
+      </c>
+      <c r="K220" s="26">
+        <v>4.3</v>
+      </c>
+      <c r="L220" s="26" t="s">
+        <v>83</v>
+      </c>
+      <c r="M220" s="26"/>
+    </row>
+    <row r="221" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A221" s="26" t="s">
+        <v>85</v>
+      </c>
+      <c r="B221" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="C221" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="D221" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="E221" s="26">
+        <v>2016</v>
+      </c>
+      <c r="F221" s="26"/>
+      <c r="G221" s="26"/>
+      <c r="H221" s="26">
+        <v>3.6</v>
+      </c>
+      <c r="I221" s="44">
+        <f>(Table1[[#This Row],[UB]]-Table1[[#This Row],[LB]])/3.92</f>
+        <v>0.30612244897959179</v>
+      </c>
+      <c r="J221" s="40">
+        <v>2.9</v>
+      </c>
+      <c r="K221" s="26">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="L221" s="26" t="s">
+        <v>83</v>
+      </c>
+      <c r="M221" s="26"/>
+    </row>
+    <row r="222" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A222" s="26" t="s">
+        <v>85</v>
+      </c>
+      <c r="B222" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="C222" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="D222" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="E222" s="26">
+        <v>2017</v>
+      </c>
+      <c r="F222" s="26"/>
+      <c r="G222" s="26"/>
+      <c r="H222" s="26">
+        <v>3.4</v>
+      </c>
+      <c r="I222" s="44">
+        <f>(Table1[[#This Row],[UB]]-Table1[[#This Row],[LB]])/3.92</f>
+        <v>0.3061224489795919</v>
+      </c>
+      <c r="J222" s="40">
+        <v>2.8</v>
+      </c>
+      <c r="K222" s="26">
+        <v>4</v>
+      </c>
+      <c r="L222" s="26" t="s">
+        <v>83</v>
+      </c>
+      <c r="M222" s="26"/>
+    </row>
+    <row r="223" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A223" s="26" t="s">
+        <v>85</v>
+      </c>
+      <c r="B223" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="C223" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="D223" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="E223" s="26">
+        <v>2018</v>
+      </c>
+      <c r="F223" s="26"/>
+      <c r="G223" s="26"/>
+      <c r="H223" s="26">
+        <v>3.3</v>
+      </c>
+      <c r="I223" s="44">
+        <f>(Table1[[#This Row],[UB]]-Table1[[#This Row],[LB]])/3.92</f>
+        <v>0.28061224489795911</v>
+      </c>
+      <c r="J223" s="40">
+        <v>2.7</v>
+      </c>
+      <c r="K223" s="26">
+        <v>3.8</v>
+      </c>
+      <c r="L223" s="26" t="s">
+        <v>83</v>
+      </c>
+      <c r="M223" s="26"/>
+    </row>
+    <row r="224" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A224" s="26" t="s">
+        <v>85</v>
+      </c>
+      <c r="B224" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="C224" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="D224" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="E224" s="26">
+        <v>2019</v>
+      </c>
+      <c r="F224" s="26"/>
+      <c r="G224" s="26"/>
+      <c r="H224" s="40">
+        <v>3.2</v>
+      </c>
+      <c r="I224" s="44">
+        <f>(Table1[[#This Row],[UB]]-Table1[[#This Row],[LB]])/3.92</f>
+        <v>0.25510204081632654</v>
+      </c>
+      <c r="J224" s="40">
+        <v>2.6</v>
+      </c>
+      <c r="K224" s="40">
+        <v>3.6</v>
+      </c>
+      <c r="L224" s="26" t="s">
+        <v>83</v>
+      </c>
+      <c r="M224" s="26"/>
+    </row>
+    <row r="225" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A225" s="41" t="s">
+        <v>90</v>
+      </c>
+      <c r="B225" s="41" t="s">
+        <v>89</v>
+      </c>
+      <c r="C225" s="41" t="s">
+        <v>59</v>
+      </c>
+      <c r="D225" s="41" t="s">
+        <v>59</v>
+      </c>
+      <c r="E225" s="41">
+        <v>1990</v>
+      </c>
+      <c r="F225" s="41"/>
+      <c r="G225" s="41"/>
+      <c r="H225" s="41">
+        <v>5.3</v>
+      </c>
+      <c r="I225" s="43">
+        <f>(Table1[[#This Row],[UB]]-Table1[[#This Row],[LB]])/3.92</f>
+        <v>0.38265306122448978</v>
+      </c>
+      <c r="J225" s="43">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="K225" s="41">
+        <v>6.1</v>
+      </c>
+      <c r="L225" s="41" t="s">
+        <v>83</v>
+      </c>
+      <c r="M225" s="41"/>
+    </row>
+    <row r="226" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A226" s="41" t="s">
+        <v>90</v>
+      </c>
+      <c r="B226" s="41" t="s">
+        <v>89</v>
+      </c>
+      <c r="C226" s="41" t="s">
+        <v>59</v>
+      </c>
+      <c r="D226" s="41" t="s">
+        <v>59</v>
+      </c>
+      <c r="E226" s="41">
+        <v>1991</v>
+      </c>
+      <c r="F226" s="41"/>
+      <c r="G226" s="41"/>
+      <c r="H226" s="41">
+        <v>6.9</v>
+      </c>
+      <c r="I226" s="43">
+        <f>(Table1[[#This Row],[UB]]-Table1[[#This Row],[LB]])/3.92</f>
+        <v>0.53571428571428559</v>
+      </c>
+      <c r="J226" s="43">
+        <v>5.9</v>
+      </c>
+      <c r="K226" s="41">
+        <v>8</v>
+      </c>
+      <c r="L226" s="41" t="s">
+        <v>83</v>
+      </c>
+      <c r="M226" s="41"/>
+    </row>
+    <row r="227" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A227" s="41" t="s">
+        <v>90</v>
+      </c>
+      <c r="B227" s="41" t="s">
+        <v>89</v>
+      </c>
+      <c r="C227" s="41" t="s">
+        <v>59</v>
+      </c>
+      <c r="D227" s="41" t="s">
+        <v>59</v>
+      </c>
+      <c r="E227" s="41">
+        <v>1992</v>
+      </c>
+      <c r="F227" s="41"/>
+      <c r="G227" s="41"/>
+      <c r="H227" s="41">
+        <v>8.5</v>
+      </c>
+      <c r="I227" s="43">
+        <f>(Table1[[#This Row],[UB]]-Table1[[#This Row],[LB]])/3.92</f>
+        <v>0.63775510204081653</v>
+      </c>
+      <c r="J227" s="43">
+        <v>7.3</v>
+      </c>
+      <c r="K227" s="41">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="L227" s="41" t="s">
+        <v>83</v>
+      </c>
+      <c r="M227" s="41"/>
+    </row>
+    <row r="228" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A228" s="41" t="s">
+        <v>90</v>
+      </c>
+      <c r="B228" s="41" t="s">
+        <v>89</v>
+      </c>
+      <c r="C228" s="41" t="s">
+        <v>59</v>
+      </c>
+      <c r="D228" s="41" t="s">
+        <v>59</v>
+      </c>
+      <c r="E228" s="41">
+        <v>1993</v>
+      </c>
+      <c r="F228" s="41"/>
+      <c r="G228" s="41"/>
+      <c r="H228" s="41">
+        <v>10</v>
+      </c>
+      <c r="I228" s="43">
+        <f>(Table1[[#This Row],[UB]]-Table1[[#This Row],[LB]])/3.92</f>
+        <v>0.73979591836734704</v>
+      </c>
+      <c r="J228" s="43">
+        <v>8.6</v>
+      </c>
+      <c r="K228" s="41">
+        <v>11.5</v>
+      </c>
+      <c r="L228" s="41" t="s">
+        <v>83</v>
+      </c>
+      <c r="M228" s="41"/>
+    </row>
+    <row r="229" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A229" s="41" t="s">
+        <v>90</v>
+      </c>
+      <c r="B229" s="41" t="s">
+        <v>89</v>
+      </c>
+      <c r="C229" s="41" t="s">
+        <v>59</v>
+      </c>
+      <c r="D229" s="41" t="s">
+        <v>59</v>
+      </c>
+      <c r="E229" s="41">
+        <v>1994</v>
+      </c>
+      <c r="F229" s="41"/>
+      <c r="G229" s="41"/>
+      <c r="H229" s="41">
+        <v>11</v>
+      </c>
+      <c r="I229" s="43">
+        <f>(Table1[[#This Row],[UB]]-Table1[[#This Row],[LB]])/3.92</f>
+        <v>0.81632653061224469</v>
+      </c>
+      <c r="J229" s="43">
+        <v>9.5</v>
+      </c>
+      <c r="K229" s="41">
+        <v>12.7</v>
+      </c>
+      <c r="L229" s="41" t="s">
+        <v>83</v>
+      </c>
+      <c r="M229" s="41"/>
+    </row>
+    <row r="230" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A230" s="41" t="s">
+        <v>90</v>
+      </c>
+      <c r="B230" s="41" t="s">
+        <v>89</v>
+      </c>
+      <c r="C230" s="41" t="s">
+        <v>59</v>
+      </c>
+      <c r="D230" s="41" t="s">
+        <v>59</v>
+      </c>
+      <c r="E230" s="41">
+        <v>1995</v>
+      </c>
+      <c r="F230" s="41"/>
+      <c r="G230" s="41"/>
+      <c r="H230" s="41">
+        <v>11.7</v>
+      </c>
+      <c r="I230" s="43">
+        <f>(Table1[[#This Row],[UB]]-Table1[[#This Row],[LB]])/3.92</f>
+        <v>0.8928571428571429</v>
+      </c>
+      <c r="J230" s="43">
+        <v>10.1</v>
+      </c>
+      <c r="K230" s="41">
+        <v>13.6</v>
+      </c>
+      <c r="L230" s="41" t="s">
+        <v>83</v>
+      </c>
+      <c r="M230" s="41"/>
+    </row>
+    <row r="231" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A231" s="41" t="s">
+        <v>90</v>
+      </c>
+      <c r="B231" s="41" t="s">
+        <v>89</v>
+      </c>
+      <c r="C231" s="41" t="s">
+        <v>59</v>
+      </c>
+      <c r="D231" s="41" t="s">
+        <v>59</v>
+      </c>
+      <c r="E231" s="41">
+        <v>1996</v>
+      </c>
+      <c r="F231" s="41"/>
+      <c r="G231" s="41"/>
+      <c r="H231" s="41">
+        <v>12</v>
+      </c>
+      <c r="I231" s="43">
+        <f>(Table1[[#This Row],[UB]]-Table1[[#This Row],[LB]])/3.92</f>
+        <v>0.8928571428571429</v>
+      </c>
+      <c r="J231" s="43">
+        <v>10.4</v>
+      </c>
+      <c r="K231" s="41">
+        <v>13.9</v>
+      </c>
+      <c r="L231" s="41" t="s">
+        <v>83</v>
+      </c>
+      <c r="M231" s="41"/>
+    </row>
+    <row r="232" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A232" s="41" t="s">
+        <v>90</v>
+      </c>
+      <c r="B232" s="41" t="s">
+        <v>89</v>
+      </c>
+      <c r="C232" s="41" t="s">
+        <v>59</v>
+      </c>
+      <c r="D232" s="41" t="s">
+        <v>59</v>
+      </c>
+      <c r="E232" s="41">
+        <v>1997</v>
+      </c>
+      <c r="F232" s="41"/>
+      <c r="G232" s="41"/>
+      <c r="H232" s="41">
+        <v>12.1</v>
+      </c>
+      <c r="I232" s="43">
+        <f>(Table1[[#This Row],[UB]]-Table1[[#This Row],[LB]])/3.92</f>
+        <v>0.8928571428571429</v>
+      </c>
+      <c r="J232" s="43">
+        <v>10.4</v>
+      </c>
+      <c r="K232" s="41">
+        <v>13.9</v>
+      </c>
+      <c r="L232" s="41" t="s">
+        <v>83</v>
+      </c>
+      <c r="M232" s="41"/>
+    </row>
+    <row r="233" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A233" s="41" t="s">
+        <v>90</v>
+      </c>
+      <c r="B233" s="41" t="s">
+        <v>89</v>
+      </c>
+      <c r="C233" s="41" t="s">
+        <v>59</v>
+      </c>
+      <c r="D233" s="41" t="s">
+        <v>59</v>
+      </c>
+      <c r="E233" s="41">
+        <v>1998</v>
+      </c>
+      <c r="F233" s="41"/>
+      <c r="G233" s="41"/>
+      <c r="H233" s="41">
+        <v>11.8</v>
+      </c>
+      <c r="I233" s="43">
+        <f>(Table1[[#This Row],[UB]]-Table1[[#This Row],[LB]])/3.92</f>
+        <v>0.8928571428571429</v>
+      </c>
+      <c r="J233" s="43">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="K233" s="41">
+        <v>13.7</v>
+      </c>
+      <c r="L233" s="41" t="s">
+        <v>83</v>
+      </c>
+      <c r="M233" s="41"/>
+    </row>
+    <row r="234" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A234" s="41" t="s">
+        <v>90</v>
+      </c>
+      <c r="B234" s="41" t="s">
+        <v>89</v>
+      </c>
+      <c r="C234" s="41" t="s">
+        <v>59</v>
+      </c>
+      <c r="D234" s="41" t="s">
+        <v>59</v>
+      </c>
+      <c r="E234" s="41">
+        <v>1999</v>
+      </c>
+      <c r="F234" s="41"/>
+      <c r="G234" s="41"/>
+      <c r="H234" s="41">
+        <v>11.5</v>
+      </c>
+      <c r="I234" s="43">
+        <f>(Table1[[#This Row],[UB]]-Table1[[#This Row],[LB]])/3.92</f>
+        <v>0.86734693877551028</v>
+      </c>
+      <c r="J234" s="43">
+        <v>9.9</v>
+      </c>
+      <c r="K234" s="41">
+        <v>13.3</v>
+      </c>
+      <c r="L234" s="41" t="s">
+        <v>83</v>
+      </c>
+      <c r="M234" s="41"/>
+    </row>
+    <row r="235" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A235" s="41" t="s">
+        <v>90</v>
+      </c>
+      <c r="B235" s="41" t="s">
+        <v>89</v>
+      </c>
+      <c r="C235" s="41" t="s">
+        <v>59</v>
+      </c>
+      <c r="D235" s="41" t="s">
+        <v>59</v>
+      </c>
+      <c r="E235" s="41">
+        <v>2000</v>
+      </c>
+      <c r="F235" s="41"/>
+      <c r="G235" s="41"/>
+      <c r="H235" s="41">
+        <v>11</v>
+      </c>
+      <c r="I235" s="43">
+        <f>(Table1[[#This Row],[UB]]-Table1[[#This Row],[LB]])/3.92</f>
+        <v>0.81632653061224469</v>
+      </c>
+      <c r="J235" s="43">
+        <v>9.5</v>
+      </c>
+      <c r="K235" s="41">
+        <v>12.7</v>
+      </c>
+      <c r="L235" s="41" t="s">
+        <v>83</v>
+      </c>
+      <c r="M235" s="41"/>
+    </row>
+    <row r="236" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A236" s="41" t="s">
+        <v>90</v>
+      </c>
+      <c r="B236" s="41" t="s">
+        <v>89</v>
+      </c>
+      <c r="C236" s="41" t="s">
+        <v>59</v>
+      </c>
+      <c r="D236" s="41" t="s">
+        <v>59</v>
+      </c>
+      <c r="E236" s="41">
+        <v>2001</v>
+      </c>
+      <c r="F236" s="41"/>
+      <c r="G236" s="41"/>
+      <c r="H236" s="41">
+        <v>10.5</v>
+      </c>
+      <c r="I236" s="43">
+        <f>(Table1[[#This Row],[UB]]-Table1[[#This Row],[LB]])/3.92</f>
+        <v>0.79081632653061218</v>
+      </c>
+      <c r="J236" s="43">
+        <v>9</v>
+      </c>
+      <c r="K236" s="41">
+        <v>12.1</v>
+      </c>
+      <c r="L236" s="41" t="s">
+        <v>83</v>
+      </c>
+      <c r="M236" s="41"/>
+    </row>
+    <row r="237" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A237" s="41" t="s">
+        <v>90</v>
+      </c>
+      <c r="B237" s="41" t="s">
+        <v>89</v>
+      </c>
+      <c r="C237" s="41" t="s">
+        <v>59</v>
+      </c>
+      <c r="D237" s="41" t="s">
+        <v>59</v>
+      </c>
+      <c r="E237" s="41">
+        <v>2002</v>
+      </c>
+      <c r="F237" s="41"/>
+      <c r="G237" s="41"/>
+      <c r="H237" s="41">
+        <v>9.9</v>
+      </c>
+      <c r="I237" s="43">
+        <f>(Table1[[#This Row],[UB]]-Table1[[#This Row],[LB]])/3.92</f>
+        <v>0.73979591836734704</v>
+      </c>
+      <c r="J237" s="43">
+        <v>8.5</v>
+      </c>
+      <c r="K237" s="41">
+        <v>11.4</v>
+      </c>
+      <c r="L237" s="41" t="s">
+        <v>83</v>
+      </c>
+      <c r="M237" s="41"/>
+    </row>
+    <row r="238" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A238" s="41" t="s">
+        <v>90</v>
+      </c>
+      <c r="B238" s="41" t="s">
+        <v>89</v>
+      </c>
+      <c r="C238" s="41" t="s">
+        <v>59</v>
+      </c>
+      <c r="D238" s="41" t="s">
+        <v>59</v>
+      </c>
+      <c r="E238" s="41">
+        <v>2003</v>
+      </c>
+      <c r="F238" s="41"/>
+      <c r="G238" s="41"/>
+      <c r="H238" s="41">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="I238" s="43">
+        <f>(Table1[[#This Row],[UB]]-Table1[[#This Row],[LB]])/3.92</f>
+        <v>0.71428571428571452</v>
+      </c>
+      <c r="J238" s="43">
+        <v>8</v>
+      </c>
+      <c r="K238" s="41">
+        <v>10.8</v>
+      </c>
+      <c r="L238" s="41" t="s">
+        <v>83</v>
+      </c>
+      <c r="M238" s="41"/>
+    </row>
+    <row r="239" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A239" s="41" t="s">
+        <v>90</v>
+      </c>
+      <c r="B239" s="41" t="s">
+        <v>89</v>
+      </c>
+      <c r="C239" s="41" t="s">
+        <v>59</v>
+      </c>
+      <c r="D239" s="41" t="s">
+        <v>59</v>
+      </c>
+      <c r="E239" s="41">
+        <v>2004</v>
+      </c>
+      <c r="F239" s="41"/>
+      <c r="G239" s="41"/>
+      <c r="H239" s="41">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="I239" s="43">
+        <f>(Table1[[#This Row],[UB]]-Table1[[#This Row],[LB]])/3.92</f>
+        <v>0.63775510204081631</v>
+      </c>
+      <c r="J239" s="43">
+        <v>7.6</v>
+      </c>
+      <c r="K239" s="41">
+        <v>10.1</v>
+      </c>
+      <c r="L239" s="41" t="s">
+        <v>83</v>
+      </c>
+      <c r="M239" s="41"/>
+    </row>
+    <row r="240" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A240" s="41" t="s">
+        <v>90</v>
+      </c>
+      <c r="B240" s="41" t="s">
+        <v>89</v>
+      </c>
+      <c r="C240" s="41" t="s">
+        <v>59</v>
+      </c>
+      <c r="D240" s="41" t="s">
+        <v>59</v>
+      </c>
+      <c r="E240" s="41">
+        <v>2005</v>
+      </c>
+      <c r="F240" s="41"/>
+      <c r="G240" s="41"/>
+      <c r="H240" s="41">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="I240" s="43">
+        <f>(Table1[[#This Row],[UB]]-Table1[[#This Row],[LB]])/3.92</f>
+        <v>0.61224489795918358</v>
+      </c>
+      <c r="J240" s="43">
+        <v>7.2</v>
+      </c>
+      <c r="K240" s="41">
+        <v>9.6</v>
+      </c>
+      <c r="L240" s="41" t="s">
+        <v>83</v>
+      </c>
+      <c r="M240" s="41"/>
+    </row>
+    <row r="241" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A241" s="41" t="s">
+        <v>90</v>
+      </c>
+      <c r="B241" s="41" t="s">
+        <v>89</v>
+      </c>
+      <c r="C241" s="41" t="s">
+        <v>59</v>
+      </c>
+      <c r="D241" s="41" t="s">
+        <v>59</v>
+      </c>
+      <c r="E241" s="41">
+        <v>2006</v>
+      </c>
+      <c r="F241" s="41"/>
+      <c r="G241" s="41"/>
+      <c r="H241" s="41">
+        <v>8</v>
+      </c>
+      <c r="I241" s="43">
+        <f>(Table1[[#This Row],[UB]]-Table1[[#This Row],[LB]])/3.92</f>
+        <v>0.58673469387755073</v>
+      </c>
+      <c r="J241" s="43">
+        <v>6.9</v>
+      </c>
+      <c r="K241" s="41">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="L241" s="41" t="s">
+        <v>83</v>
+      </c>
+      <c r="M241" s="41"/>
+    </row>
+    <row r="242" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A242" s="41" t="s">
+        <v>90</v>
+      </c>
+      <c r="B242" s="41" t="s">
+        <v>89</v>
+      </c>
+      <c r="C242" s="41" t="s">
+        <v>59</v>
+      </c>
+      <c r="D242" s="41" t="s">
+        <v>59</v>
+      </c>
+      <c r="E242" s="41">
+        <v>2007</v>
+      </c>
+      <c r="F242" s="41"/>
+      <c r="G242" s="41"/>
+      <c r="H242" s="41">
+        <v>7.7</v>
+      </c>
+      <c r="I242" s="43">
+        <f>(Table1[[#This Row],[UB]]-Table1[[#This Row],[LB]])/3.92</f>
+        <v>0.58673469387755117</v>
+      </c>
+      <c r="J242" s="43">
+        <v>6.6</v>
+      </c>
+      <c r="K242" s="41">
+        <v>8.9</v>
+      </c>
+      <c r="L242" s="41" t="s">
+        <v>83</v>
+      </c>
+      <c r="M242" s="41"/>
+    </row>
+    <row r="243" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A243" s="41" t="s">
+        <v>90</v>
+      </c>
+      <c r="B243" s="41" t="s">
+        <v>89</v>
+      </c>
+      <c r="C243" s="41" t="s">
+        <v>59</v>
+      </c>
+      <c r="D243" s="41" t="s">
+        <v>59</v>
+      </c>
+      <c r="E243" s="41">
+        <v>2008</v>
+      </c>
+      <c r="F243" s="41"/>
+      <c r="G243" s="41"/>
+      <c r="H243" s="41">
+        <v>7.5</v>
+      </c>
+      <c r="I243" s="43">
+        <f>(Table1[[#This Row],[UB]]-Table1[[#This Row],[LB]])/3.92</f>
+        <v>0.56122448979591821</v>
+      </c>
+      <c r="J243" s="43">
+        <v>6.4</v>
+      </c>
+      <c r="K243" s="41">
+        <v>8.6</v>
+      </c>
+      <c r="L243" s="41" t="s">
+        <v>83</v>
+      </c>
+      <c r="M243" s="41"/>
+    </row>
+    <row r="244" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A244" s="41" t="s">
+        <v>90</v>
+      </c>
+      <c r="B244" s="41" t="s">
+        <v>89</v>
+      </c>
+      <c r="C244" s="41" t="s">
+        <v>59</v>
+      </c>
+      <c r="D244" s="41" t="s">
+        <v>59</v>
+      </c>
+      <c r="E244" s="41">
+        <v>2009</v>
+      </c>
+      <c r="F244" s="41"/>
+      <c r="G244" s="41"/>
+      <c r="H244" s="41">
+        <v>7.3</v>
+      </c>
+      <c r="I244" s="43">
+        <f>(Table1[[#This Row],[UB]]-Table1[[#This Row],[LB]])/3.92</f>
+        <v>0.53571428571428581</v>
+      </c>
+      <c r="J244" s="43">
+        <v>6.3</v>
+      </c>
+      <c r="K244" s="41">
+        <v>8.4</v>
+      </c>
+      <c r="L244" s="41" t="s">
+        <v>83</v>
+      </c>
+      <c r="M244" s="41"/>
+    </row>
+    <row r="245" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A245" s="41" t="s">
+        <v>90</v>
+      </c>
+      <c r="B245" s="41" t="s">
+        <v>89</v>
+      </c>
+      <c r="C245" s="41" t="s">
+        <v>59</v>
+      </c>
+      <c r="D245" s="41" t="s">
+        <v>59</v>
+      </c>
+      <c r="E245" s="41">
+        <v>2010</v>
+      </c>
+      <c r="F245" s="41"/>
+      <c r="G245" s="41"/>
+      <c r="H245" s="41">
+        <v>7.2</v>
+      </c>
+      <c r="I245" s="43">
+        <f>(Table1[[#This Row],[UB]]-Table1[[#This Row],[LB]])/3.92</f>
+        <v>0.53571428571428581</v>
+      </c>
+      <c r="J245" s="43">
+        <v>6.2</v>
+      </c>
+      <c r="K245" s="41">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="L245" s="41" t="s">
+        <v>83</v>
+      </c>
+      <c r="M245" s="41"/>
+    </row>
+    <row r="246" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A246" s="41" t="s">
+        <v>90</v>
+      </c>
+      <c r="B246" s="41" t="s">
+        <v>89</v>
+      </c>
+      <c r="C246" s="41" t="s">
+        <v>59</v>
+      </c>
+      <c r="D246" s="41" t="s">
+        <v>59</v>
+      </c>
+      <c r="E246" s="41">
+        <v>2011</v>
+      </c>
+      <c r="F246" s="41"/>
+      <c r="G246" s="41"/>
+      <c r="H246" s="41">
+        <v>7</v>
+      </c>
+      <c r="I246" s="43">
+        <f>(Table1[[#This Row],[UB]]-Table1[[#This Row],[LB]])/3.92</f>
+        <v>0.53571428571428559</v>
+      </c>
+      <c r="J246" s="43">
+        <v>6</v>
+      </c>
+      <c r="K246" s="41">
+        <v>8.1</v>
+      </c>
+      <c r="L246" s="41" t="s">
+        <v>83</v>
+      </c>
+      <c r="M246" s="41"/>
+    </row>
+    <row r="247" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A247" s="41" t="s">
+        <v>90</v>
+      </c>
+      <c r="B247" s="41" t="s">
+        <v>89</v>
+      </c>
+      <c r="C247" s="41" t="s">
+        <v>59</v>
+      </c>
+      <c r="D247" s="41" t="s">
+        <v>59</v>
+      </c>
+      <c r="E247" s="41">
+        <v>2012</v>
+      </c>
+      <c r="F247" s="41"/>
+      <c r="G247" s="41"/>
+      <c r="H247" s="41">
+        <v>6.9</v>
+      </c>
+      <c r="I247" s="43">
+        <f>(Table1[[#This Row],[UB]]-Table1[[#This Row],[LB]])/3.92</f>
+        <v>0.53571428571428559</v>
+      </c>
+      <c r="J247" s="43">
+        <v>5.9</v>
+      </c>
+      <c r="K247" s="41">
+        <v>8</v>
+      </c>
+      <c r="L247" s="41" t="s">
+        <v>83</v>
+      </c>
+      <c r="M247" s="41"/>
+    </row>
+    <row r="248" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A248" s="41" t="s">
+        <v>90</v>
+      </c>
+      <c r="B248" s="41" t="s">
+        <v>89</v>
+      </c>
+      <c r="C248" s="41" t="s">
+        <v>59</v>
+      </c>
+      <c r="D248" s="41" t="s">
+        <v>59</v>
+      </c>
+      <c r="E248" s="41">
+        <v>2013</v>
+      </c>
+      <c r="F248" s="41"/>
+      <c r="G248" s="41"/>
+      <c r="H248" s="41">
+        <v>6.8</v>
+      </c>
+      <c r="I248" s="43">
+        <f>(Table1[[#This Row],[UB]]-Table1[[#This Row],[LB]])/3.92</f>
+        <v>0.51020408163265307</v>
+      </c>
+      <c r="J248" s="43">
+        <v>5.8</v>
+      </c>
+      <c r="K248" s="41">
+        <v>7.8</v>
+      </c>
+      <c r="L248" s="41" t="s">
+        <v>83</v>
+      </c>
+      <c r="M248" s="41"/>
+    </row>
+    <row r="249" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A249" s="41" t="s">
+        <v>90</v>
+      </c>
+      <c r="B249" s="41" t="s">
+        <v>89</v>
+      </c>
+      <c r="C249" s="41" t="s">
+        <v>59</v>
+      </c>
+      <c r="D249" s="41" t="s">
+        <v>59</v>
+      </c>
+      <c r="E249" s="41">
+        <v>2014</v>
+      </c>
+      <c r="F249" s="41"/>
+      <c r="G249" s="41"/>
+      <c r="H249" s="41">
+        <v>6.7</v>
+      </c>
+      <c r="I249" s="43">
+        <f>(Table1[[#This Row],[UB]]-Table1[[#This Row],[LB]])/3.92</f>
+        <v>0.51020408163265307</v>
+      </c>
+      <c r="J249" s="43">
+        <v>5.7</v>
+      </c>
+      <c r="K249" s="41">
+        <v>7.7</v>
+      </c>
+      <c r="L249" s="41" t="s">
+        <v>83</v>
+      </c>
+      <c r="M249" s="41"/>
+    </row>
+    <row r="250" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A250" s="41" t="s">
+        <v>90</v>
+      </c>
+      <c r="B250" s="41" t="s">
+        <v>89</v>
+      </c>
+      <c r="C250" s="41" t="s">
+        <v>59</v>
+      </c>
+      <c r="D250" s="41" t="s">
+        <v>59</v>
+      </c>
+      <c r="E250" s="41">
+        <v>2015</v>
+      </c>
+      <c r="F250" s="41"/>
+      <c r="G250" s="41"/>
+      <c r="H250" s="41">
+        <v>6.5</v>
+      </c>
+      <c r="I250" s="43">
+        <f>(Table1[[#This Row],[UB]]-Table1[[#This Row],[LB]])/3.92</f>
+        <v>0.4846938775510205</v>
+      </c>
+      <c r="J250" s="43">
+        <v>5.6</v>
+      </c>
+      <c r="K250" s="41">
+        <v>7.5</v>
+      </c>
+      <c r="L250" s="41" t="s">
+        <v>83</v>
+      </c>
+      <c r="M250" s="41"/>
+    </row>
+    <row r="251" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A251" s="41" t="s">
+        <v>90</v>
+      </c>
+      <c r="B251" s="41" t="s">
+        <v>89</v>
+      </c>
+      <c r="C251" s="41" t="s">
+        <v>59</v>
+      </c>
+      <c r="D251" s="41" t="s">
+        <v>59</v>
+      </c>
+      <c r="E251" s="41">
+        <v>2016</v>
+      </c>
+      <c r="F251" s="41"/>
+      <c r="G251" s="41"/>
+      <c r="H251" s="41">
+        <v>6.4</v>
+      </c>
+      <c r="I251" s="43">
+        <f>(Table1[[#This Row],[UB]]-Table1[[#This Row],[LB]])/3.92</f>
+        <v>0.4846938775510205</v>
+      </c>
+      <c r="J251" s="43">
+        <v>5.5</v>
+      </c>
+      <c r="K251" s="41">
+        <v>7.4</v>
+      </c>
+      <c r="L251" s="41" t="s">
+        <v>83</v>
+      </c>
+      <c r="M251" s="41"/>
+    </row>
+    <row r="252" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A252" s="41" t="s">
+        <v>90</v>
+      </c>
+      <c r="B252" s="41" t="s">
+        <v>89</v>
+      </c>
+      <c r="C252" s="41" t="s">
+        <v>59</v>
+      </c>
+      <c r="D252" s="41" t="s">
+        <v>59</v>
+      </c>
+      <c r="E252" s="41">
+        <v>2017</v>
+      </c>
+      <c r="F252" s="41"/>
+      <c r="G252" s="41"/>
+      <c r="H252" s="41">
+        <v>6.2</v>
+      </c>
+      <c r="I252" s="43">
+        <f>(Table1[[#This Row],[UB]]-Table1[[#This Row],[LB]])/3.92</f>
+        <v>0.4846938775510205</v>
+      </c>
+      <c r="J252" s="43">
+        <v>5.3</v>
+      </c>
+      <c r="K252" s="41">
+        <v>7.2</v>
+      </c>
+      <c r="L252" s="41" t="s">
+        <v>83</v>
+      </c>
+      <c r="M252" s="41"/>
+    </row>
+    <row r="253" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A253" s="41" t="s">
+        <v>90</v>
+      </c>
+      <c r="B253" s="41" t="s">
+        <v>89</v>
+      </c>
+      <c r="C253" s="41" t="s">
+        <v>59</v>
+      </c>
+      <c r="D253" s="41" t="s">
+        <v>59</v>
+      </c>
+      <c r="E253" s="41">
+        <v>2018</v>
+      </c>
+      <c r="F253" s="41"/>
+      <c r="G253" s="41"/>
+      <c r="H253" s="41">
+        <v>6</v>
+      </c>
+      <c r="I253" s="43">
+        <f>(Table1[[#This Row],[UB]]-Table1[[#This Row],[LB]])/3.92</f>
+        <v>0.45918367346938771</v>
+      </c>
+      <c r="J253" s="43">
+        <v>5.2</v>
+      </c>
+      <c r="K253" s="41">
+        <v>7</v>
+      </c>
+      <c r="L253" s="41" t="s">
+        <v>83</v>
+      </c>
+      <c r="M253" s="41"/>
+    </row>
+    <row r="254" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A254" s="41" t="s">
+        <v>90</v>
+      </c>
+      <c r="B254" s="41" t="s">
+        <v>89</v>
+      </c>
+      <c r="C254" s="41" t="s">
+        <v>59</v>
+      </c>
+      <c r="D254" s="41" t="s">
+        <v>59</v>
+      </c>
+      <c r="E254" s="41">
+        <v>2019</v>
+      </c>
+      <c r="F254" s="41"/>
+      <c r="G254" s="41"/>
+      <c r="H254" s="41">
+        <v>5.8</v>
+      </c>
+      <c r="I254" s="43">
+        <f>(Table1[[#This Row],[UB]]-Table1[[#This Row],[LB]])/3.92</f>
+        <v>0.43367346938775514</v>
+      </c>
+      <c r="J254" s="41">
+        <v>5</v>
+      </c>
+      <c r="K254" s="41">
+        <v>6.7</v>
+      </c>
+      <c r="L254" s="41" t="s">
+        <v>83</v>
+      </c>
+      <c r="M254" s="41"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updates based on recalibration of kSymp using a random probability from Cari's prior distributions.
</commit_message>
<xml_diff>
--- a/Config/Calibration_targets_Kenya.xlsx
+++ b/Config/Calibration_targets_Kenya.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10709"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clh89/MATLAB/Projects/Kenya_treatment/Config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8100F71B-A7CA-B041-869D-E52E28DF66BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0D87ABD-9465-C245-821A-C43E3FC9A469}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-33160" yWindow="-1960" windowWidth="30720" windowHeight="17900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="779" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="782" uniqueCount="91">
   <si>
     <t>Criteria</t>
   </si>
@@ -306,6 +306,9 @@
   </si>
   <si>
     <t>Mungo 2021</t>
+  </si>
+  <si>
+    <t>2017-2020</t>
   </si>
 </sst>
 </file>
@@ -833,8 +836,8 @@
   <dimension ref="A1:M177"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A160" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J182" sqref="J182"/>
+      <pane ySplit="1" topLeftCell="A164" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E175" sqref="E175:E177"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7189,8 +7192,8 @@
       <c r="D175" t="s">
         <v>59</v>
       </c>
-      <c r="E175">
-        <v>2018</v>
+      <c r="E175" t="s">
+        <v>90</v>
       </c>
       <c r="H175">
         <f>(3+20)/(3+20+10+28+7+27+7+6)</f>
@@ -7216,8 +7219,8 @@
       <c r="D176" t="s">
         <v>88</v>
       </c>
-      <c r="E176">
-        <v>2018</v>
+      <c r="E176" t="s">
+        <v>90</v>
       </c>
       <c r="H176">
         <f>(10+28+7+27)/(3+20+10+28+7+27+7+6)</f>
@@ -7243,8 +7246,8 @@
       <c r="D177" t="s">
         <v>88</v>
       </c>
-      <c r="E177">
-        <v>2018</v>
+      <c r="E177" t="s">
+        <v>90</v>
       </c>
       <c r="H177">
         <v>0.12037037037037046</v>

</xml_diff>